<commit_message>
actualizar documento: capítulos 3 y 4
</commit_message>
<xml_diff>
--- a/documento/tablas/tablas_tfm.xlsx
+++ b/documento/tablas/tablas_tfm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Dropbox/Transporte_interno/Máster/Ciencia de Datos/TFM/documento/tablas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C983F8-FDFC-D04C-B866-4C7281474E8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC87E38-10B9-334D-9CA9-63C2B7A377B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="2040" windowWidth="26680" windowHeight="17920" tabRatio="752" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6920" yWindow="2040" windowWidth="26680" windowHeight="17920" tabRatio="752" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="10" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="254">
   <si>
     <t>Grupo de edad</t>
   </si>
@@ -1443,7 +1443,7 @@
   <dimension ref="B2:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F21" sqref="F21:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1552,7 +1552,7 @@
         <v>219</v>
       </c>
       <c r="G8" s="35" t="str">
-        <f t="shared" ref="G8:G34" si="1">C8 &amp; " (" &amp; ROUND(100*D8,1) &amp; "%)"</f>
+        <f t="shared" ref="G8:G20" si="1">C8 &amp; " (" &amp; ROUND(100*D8,1) &amp; "%)"</f>
         <v>34 (8,4%)</v>
       </c>
     </row>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="D21" s="37"/>
       <c r="F21" s="38" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="G21" s="35"/>
     </row>
@@ -1796,11 +1796,11 @@
         <v>4.9504950495049507E-2</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="G22" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>20 (5%)</v>
+        <f>C26 &amp; " (" &amp; ROUND(100*D26,1) &amp; "%)"</f>
+        <v>212 (52,5%)</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
@@ -1815,11 +1815,11 @@
         <v>0.90346534653465349</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G23" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>365 (90,3%)</v>
+        <f>C27 &amp; " (" &amp; ROUND(100*D27,1) &amp; "%)"</f>
+        <v>161 (39,9%)</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
@@ -1834,10 +1834,10 @@
         <v>4.702970297029703E-2</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="G24" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f>C28 &amp; " (" &amp; ROUND(100*D28,1) &amp; "%)"</f>
         <v>19 (4,7%)</v>
       </c>
     </row>
@@ -1846,10 +1846,13 @@
         <v>230</v>
       </c>
       <c r="D25" s="37"/>
-      <c r="F25" s="38" t="s">
-        <v>230</v>
-      </c>
-      <c r="G25" s="35"/>
+      <c r="F25" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="G25" s="35" t="str">
+        <f>C29 &amp; " (" &amp; ROUND(100*D29,1) &amp; "%)"</f>
+        <v>10 (2,5%)</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="35" t="s">
@@ -1863,11 +1866,11 @@
         <v>0.52475247524752477</v>
       </c>
       <c r="F26" s="35" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G26" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>212 (52,5%)</v>
+        <f>C30 &amp; " (" &amp; ROUND(100*D30,1) &amp; "%)"</f>
+        <v>2 (0,5%)</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
@@ -1881,13 +1884,10 @@
         <f t="shared" si="2"/>
         <v>0.39851485148514854</v>
       </c>
-      <c r="F27" s="35" t="s">
-        <v>232</v>
-      </c>
-      <c r="G27" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>161 (39,9%)</v>
-      </c>
+      <c r="F27" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="G27" s="35"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="35" t="s">
@@ -1901,11 +1901,11 @@
         <v>4.702970297029703E-2</v>
       </c>
       <c r="F28" s="35" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="G28" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>19 (4,7%)</v>
+        <f>C32 &amp; " (" &amp; ROUND(100*D32,1) &amp; "%)"</f>
+        <v>257 (63,6%)</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
@@ -1920,11 +1920,11 @@
         <v>2.4752475247524754E-2</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="G29" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>10 (2,5%)</v>
+        <f>C33 &amp; " (" &amp; ROUND(100*D33,1) &amp; "%)"</f>
+        <v>146 (36,1%)</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
@@ -1939,11 +1939,11 @@
         <v>4.9504950495049506E-3</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="G30" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>2 (0,5%)</v>
+        <f>C34 &amp; " (" &amp; ROUND(100*D34,1) &amp; "%)"</f>
+        <v>1 (0,2%)</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
@@ -1951,10 +1951,6 @@
         <v>235</v>
       </c>
       <c r="D31" s="37"/>
-      <c r="F31" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="G31" s="35"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" s="35" t="s">
@@ -1967,15 +1963,8 @@
         <f t="shared" si="2"/>
         <v>0.63613861386138615</v>
       </c>
-      <c r="F32" s="35" t="s">
-        <v>236</v>
-      </c>
-      <c r="G32" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>257 (63,6%)</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="35" t="s">
         <v>248</v>
       </c>
@@ -1986,15 +1975,8 @@
         <f t="shared" si="2"/>
         <v>0.36138613861386137</v>
       </c>
-      <c r="F33" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="G33" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>146 (36,1%)</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="35" t="s">
         <v>217</v>
       </c>
@@ -2004,13 +1986,6 @@
       <c r="D34" s="37">
         <f t="shared" si="2"/>
         <v>2.4752475247524753E-3</v>
-      </c>
-      <c r="F34" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="G34" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>1 (0,2%)</v>
       </c>
     </row>
   </sheetData>
@@ -2536,8 +2511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9964D0ED-D39A-9F40-BAAC-91509B1851FE}">
   <dimension ref="B1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2650,7 +2625,7 @@
         <v>219</v>
       </c>
       <c r="G8" s="35" t="str">
-        <f t="shared" ref="G8:G33" si="1">C8 &amp; " (" &amp; ROUND(100*D8,1) &amp; "%)"</f>
+        <f t="shared" ref="G8:G20" si="1">C8 &amp; " (" &amp; ROUND(100*D8,1) &amp; "%)"</f>
         <v>16 (2,6%)</v>
       </c>
     </row>
@@ -2878,7 +2853,7 @@
       </c>
       <c r="D21" s="37"/>
       <c r="F21" s="38" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="G21" s="35"/>
     </row>
@@ -2894,11 +2869,11 @@
         <v>8.0645161290322578E-3</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="G22" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>5 (0,8%)</v>
+        <f>C26 &amp; " (" &amp; ROUND(100*D26,1) &amp; "%)"</f>
+        <v>293 (47,3%)</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
@@ -2913,11 +2888,11 @@
         <v>0.56774193548387097</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G23" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>352 (56,8%)</v>
+        <f>C27 &amp; " (" &amp; ROUND(100*D27,1) &amp; "%)"</f>
+        <v>13 (2,1%)</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
@@ -2931,12 +2906,12 @@
         <f t="shared" si="2"/>
         <v>0.42419354838709677</v>
       </c>
-      <c r="F24" s="45" t="s">
-        <v>217</v>
-      </c>
-      <c r="G24" s="45" t="str">
-        <f t="shared" si="1"/>
-        <v>263 (42,4%)</v>
+      <c r="F24" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="G24" s="35" t="str">
+        <f>C28 &amp; " (" &amp; ROUND(100*D28,1) &amp; "%)"</f>
+        <v>65 (10,5%)</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
@@ -2944,10 +2919,13 @@
         <v>230</v>
       </c>
       <c r="D25" s="37"/>
-      <c r="F25" s="38" t="s">
-        <v>230</v>
-      </c>
-      <c r="G25" s="35"/>
+      <c r="F25" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="G25" s="35" t="str">
+        <f>C29 &amp; " (" &amp; ROUND(100*D29,1) &amp; "%)"</f>
+        <v>248 (40%)</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="35" t="s">
@@ -2960,12 +2938,12 @@
         <f t="shared" si="2"/>
         <v>0.47258064516129034</v>
       </c>
-      <c r="F26" s="35" t="s">
-        <v>233</v>
-      </c>
-      <c r="G26" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>293 (47,3%)</v>
+      <c r="F26" s="45" t="s">
+        <v>231</v>
+      </c>
+      <c r="G26" s="45" t="str">
+        <f>C30 &amp; " (" &amp; ROUND(100*D30,1) &amp; "%)"</f>
+        <v>1 (0,2%)</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
@@ -2979,13 +2957,10 @@
         <f t="shared" si="2"/>
         <v>2.0967741935483872E-2</v>
       </c>
-      <c r="F27" s="35" t="s">
-        <v>232</v>
-      </c>
-      <c r="G27" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>13 (2,1%)</v>
-      </c>
+      <c r="F27" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="G27" s="35"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="35" t="s">
@@ -2999,11 +2974,11 @@
         <v>0.10483870967741936</v>
       </c>
       <c r="F28" s="35" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="G28" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>65 (10,5%)</v>
+        <f>C32 &amp; " (" &amp; ROUND(100*D32,1) &amp; "%)"</f>
+        <v>491 (79,2%)</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
@@ -3017,12 +2992,12 @@
         <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="F29" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="G29" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>248 (40%)</v>
+      <c r="F29" s="45" t="s">
+        <v>237</v>
+      </c>
+      <c r="G29" s="45" t="str">
+        <f>C33 &amp; " (" &amp; ROUND(100*D33,1) &amp; "%)"</f>
+        <v>129 (20,8%)</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
@@ -3036,23 +3011,12 @@
         <f t="shared" si="2"/>
         <v>1.6129032258064516E-3</v>
       </c>
-      <c r="F30" s="45" t="s">
-        <v>231</v>
-      </c>
-      <c r="G30" s="45" t="str">
-        <f t="shared" si="1"/>
-        <v>1 (0,2%)</v>
-      </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" s="38" t="s">
         <v>235</v>
       </c>
       <c r="D31" s="37"/>
-      <c r="F31" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="G31" s="35"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" s="35" t="s">
@@ -3065,15 +3029,8 @@
         <f t="shared" si="2"/>
         <v>0.79193548387096779</v>
       </c>
-      <c r="F32" s="35" t="s">
-        <v>236</v>
-      </c>
-      <c r="G32" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>491 (79,2%)</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="35" t="s">
         <v>248</v>
       </c>
@@ -3083,13 +3040,6 @@
       <c r="D33" s="37">
         <f t="shared" si="2"/>
         <v>0.20806451612903226</v>
-      </c>
-      <c r="F33" s="45" t="s">
-        <v>237</v>
-      </c>
-      <c r="G33" s="45" t="str">
-        <f t="shared" si="1"/>
-        <v>129 (20,8%)</v>
       </c>
     </row>
   </sheetData>
@@ -7216,7 +7166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B244C3-CB16-495F-980A-6CB4471F2FAB}">
   <dimension ref="A3:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
actualizar documento - borrador 26-Jul-2020
</commit_message>
<xml_diff>
--- a/documento/tablas/tablas_tfm.xlsx
+++ b/documento/tablas/tablas_tfm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Dropbox/Transporte_interno/Máster/Ciencia de Datos/TFM/documento/tablas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3F1BD7-2E69-6448-BF9D-C7E1B7AEE539}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14770258-47D3-BA45-97CD-EB0397444F27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1780" windowWidth="17800" windowHeight="17920" tabRatio="752" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="4040" windowWidth="15880" windowHeight="13940" tabRatio="752" firstSheet="24" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Poblaciones estándar" sheetId="19" r:id="rId1"/>
@@ -21,14 +21,30 @@
     <sheet name="6 - Mortalidad hígado" sheetId="24" r:id="rId6"/>
     <sheet name="7 - Mortalidad CR" sheetId="25" r:id="rId7"/>
     <sheet name="8 - Prevalencia" sheetId="26" r:id="rId8"/>
-    <sheet name="Matriz de confusión" sheetId="36" r:id="rId9"/>
+    <sheet name="SN -  Matriz de confusión" sheetId="36" r:id="rId9"/>
     <sheet name="9 - Hígado datos clínicos" sheetId="27" r:id="rId10"/>
     <sheet name="10 - Hígado estado vital" sheetId="28" r:id="rId11"/>
     <sheet name="11 - CR datos clínicos" sheetId="29" r:id="rId12"/>
     <sheet name="12 - CR estado vital" sheetId="30" r:id="rId13"/>
-    <sheet name="13 - Tipo de muestra HB " sheetId="33" r:id="rId14"/>
-    <sheet name="14 - train-test HB" sheetId="35" r:id="rId15"/>
-    <sheet name="15 - Genes HB" sheetId="31" r:id="rId16"/>
+    <sheet name="13 - parámetros SVM tuning" sheetId="38" r:id="rId14"/>
+    <sheet name="14 - Tipo de muestra HB " sheetId="33" r:id="rId15"/>
+    <sheet name="15 - train-test HB" sheetId="35" r:id="rId16"/>
+    <sheet name="16 - Genes HB" sheetId="31" r:id="rId17"/>
+    <sheet name="17 - tuningSVM HB" sheetId="39" r:id="rId18"/>
+    <sheet name="18 - tuningkNN HB" sheetId="40" r:id="rId19"/>
+    <sheet name="19 - Mejores modelos HB" sheetId="37" r:id="rId20"/>
+    <sheet name="20 - tipo de muestra HM" sheetId="42" r:id="rId21"/>
+    <sheet name="21 - train-test HM" sheetId="43" r:id="rId22"/>
+    <sheet name="22 - genes HM" sheetId="44" r:id="rId23"/>
+    <sheet name="23 - tuningSVM HM" sheetId="45" r:id="rId24"/>
+    <sheet name="24 - tuning kNN HM" sheetId="47" r:id="rId25"/>
+    <sheet name="25 - mejores modelos HM" sheetId="46" r:id="rId26"/>
+    <sheet name="26 - tipo de muestra CRB" sheetId="48" r:id="rId27"/>
+    <sheet name="27 - traintest CRB" sheetId="49" r:id="rId28"/>
+    <sheet name="28 - genes CRB" sheetId="50" r:id="rId29"/>
+    <sheet name="29 - tuningSVM CRB" sheetId="51" r:id="rId30"/>
+    <sheet name="30 - tuningkNN CRB" sheetId="52" r:id="rId31"/>
+    <sheet name="31 - mejores modelos CRB" sheetId="53" r:id="rId32"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="411">
   <si>
     <t>Grupo de edad</t>
   </si>
@@ -947,16 +963,361 @@
   </si>
   <si>
     <t>Falsos negativos (FN)</t>
+  </si>
+  <si>
+    <t>Biclase</t>
+  </si>
+  <si>
+    <t>Parámetros</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>RF 4 genes</t>
+  </si>
+  <si>
+    <t>mRMR 7 genes</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>kNN</t>
+  </si>
+  <si>
+    <t>RF 2 genes</t>
+  </si>
+  <si>
+    <t>http://onlineconfusionmatrix.com</t>
+  </si>
+  <si>
+    <t>Multiclase morfología</t>
+  </si>
+  <si>
+    <t>coste = 1
+gamma = 0.025</t>
+  </si>
+  <si>
+    <t>mRMR 6 genes</t>
+  </si>
+  <si>
+    <t>90,63</t>
+  </si>
+  <si>
+    <t>mRmR 7 genes</t>
+  </si>
+  <si>
+    <t>k = 7</t>
+  </si>
+  <si>
+    <t>Multiclase estadio</t>
+  </si>
+  <si>
+    <t>mrmr 5 genes</t>
+  </si>
+  <si>
+    <t>coste = 0.05
+gamma = 0.05</t>
+  </si>
+  <si>
+    <t>mrmr 7 genes</t>
+  </si>
+  <si>
+    <t>63,20</t>
+  </si>
+  <si>
+    <t>mrmr 1 gen</t>
+  </si>
+  <si>
+    <t>k = 9</t>
+  </si>
+  <si>
+    <t>78,10</t>
+  </si>
+  <si>
+    <t>Coste</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Biomarcadores</t>
+  </si>
+  <si>
+    <t>$c$ = 0.75
+$\gamma$ = 0.1</t>
+  </si>
+  <si>
+    <t>$k$ = 5</t>
+  </si>
+  <si>
+    <t>F1 train</t>
+  </si>
+  <si>
+    <t>Acc train</t>
+  </si>
+  <si>
+    <t>F1 test</t>
+  </si>
+  <si>
+    <t>Acc test</t>
+  </si>
+  <si>
+    <t>44 (75,9%)</t>
+  </si>
+  <si>
+    <t>14 (24,1%)</t>
+  </si>
+  <si>
+    <t>363 (100%)</t>
+  </si>
+  <si>
+    <t>33 (100%)</t>
+  </si>
+  <si>
+    <t>Proporción
+colang./sanos</t>
+  </si>
+  <si>
+    <t>Proporción
+carc. hepat./sanos</t>
+  </si>
+  <si>
+    <t>273 (75,2%)</t>
+  </si>
+  <si>
+    <t>25 (75,8%)</t>
+  </si>
+  <si>
+    <t>90 (24,8%)</t>
+  </si>
+  <si>
+    <t>8 (24,2%)</t>
+  </si>
+  <si>
+    <t>WWTR1</t>
+  </si>
+  <si>
+    <t>FTLP3</t>
+  </si>
+  <si>
+    <t>BIRC3</t>
+  </si>
+  <si>
+    <t>PLXDC1</t>
+  </si>
+  <si>
+    <t>CDH1</t>
+  </si>
+  <si>
+    <t>RAB25</t>
+  </si>
+  <si>
+    <t>STAB2</t>
+  </si>
+  <si>
+    <t>ROS1</t>
+  </si>
+  <si>
+    <t>WDR66</t>
+  </si>
+  <si>
+    <t>POLQ</t>
+  </si>
+  <si>
+    <t>AP2B1</t>
+  </si>
+  <si>
+    <t>ECM1</t>
+  </si>
+  <si>
+    <t>FGFR2</t>
+  </si>
+  <si>
+    <t>KLF6</t>
+  </si>
+  <si>
+    <t>PTPN13</t>
+  </si>
+  <si>
+    <t>GDF2</t>
+  </si>
+  <si>
+    <t>CBFB</t>
+  </si>
+  <si>
+    <t>SLC31A1</t>
+  </si>
+  <si>
+    <t>FGFR3</t>
+  </si>
+  <si>
+    <t>SPDL1</t>
+  </si>
+  <si>
+    <t>CLTCL1</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>mrmr</t>
+  </si>
+  <si>
+    <t>rf</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>$c$ = 1
+$\gamma$ = 0.025</t>
+  </si>
+  <si>
+    <t>Tumor</t>
+  </si>
+  <si>
+    <t>644 (100%)</t>
+  </si>
+  <si>
+    <t>51 (100%)</t>
+  </si>
+  <si>
+    <t>483 (75,0%)</t>
+  </si>
+  <si>
+    <t>39 (76,5%)</t>
+  </si>
+  <si>
+    <t>161 (25,0%)</t>
+  </si>
+  <si>
+    <t>12 (23,5%)</t>
+  </si>
+  <si>
+    <t>BEST4</t>
+  </si>
+  <si>
+    <t>VSTM2A</t>
+  </si>
+  <si>
+    <t>ETV4</t>
+  </si>
+  <si>
+    <t>MET</t>
+  </si>
+  <si>
+    <t>CA7</t>
+  </si>
+  <si>
+    <t>SCN7A</t>
+  </si>
+  <si>
+    <t>EPOP</t>
+  </si>
+  <si>
+    <t>COL11A1</t>
+  </si>
+  <si>
+    <t>RSPO2</t>
+  </si>
+  <si>
+    <t>RXRG</t>
+  </si>
+  <si>
+    <t>GLP2R</t>
+  </si>
+  <si>
+    <t>PHOX2B</t>
+  </si>
+  <si>
+    <t>C5orf34</t>
+  </si>
+  <si>
+    <t>SLC39A10</t>
+  </si>
+  <si>
+    <t>SALL4</t>
+  </si>
+  <si>
+    <t>DHRS7C</t>
+  </si>
+  <si>
+    <t>ENC1</t>
+  </si>
+  <si>
+    <t>POU5F1B</t>
+  </si>
+  <si>
+    <t>NKX2-3</t>
+  </si>
+  <si>
+    <t>ESM1</t>
+  </si>
+  <si>
+    <t>TNFRSF17</t>
+  </si>
+  <si>
+    <t>CEMIP</t>
+  </si>
+  <si>
+    <t>SCN9A</t>
+  </si>
+  <si>
+    <t>SGCG</t>
+  </si>
+  <si>
+    <t>CA2</t>
+  </si>
+  <si>
+    <t>TLX1</t>
+  </si>
+  <si>
+    <t>MDFI</t>
+  </si>
+  <si>
+    <t>KRT80</t>
+  </si>
+  <si>
+    <t>WT1</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>mRMR 3 genes</t>
+  </si>
+  <si>
+    <t>RF 3 genes</t>
+  </si>
+  <si>
+    <t>$c$ = 0,05
+$\gamma$ = 0,06</t>
+  </si>
+  <si>
+    <t>$c$ = 0,05
+$\gamma$ = 0,07</t>
+  </si>
+  <si>
+    <t>k = 23</t>
+  </si>
+  <si>
+    <t>mRMR 4 genes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1028,6 +1389,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1043,7 +1426,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1090,13 +1473,354 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1258,14 +1982,192 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -3004,14 +3906,14 @@
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="109" t="s">
         <v>229</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62" t="s">
+      <c r="D2" s="109"/>
+      <c r="E2" s="109" t="s">
         <v>230</v>
       </c>
-      <c r="F2" s="62"/>
+      <c r="F2" s="109"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="34" t="s">
@@ -4182,14 +5084,14 @@
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="109" t="s">
         <v>229</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62" t="s">
+      <c r="D2" s="109"/>
+      <c r="E2" s="109" t="s">
         <v>230</v>
       </c>
-      <c r="F2" s="62"/>
+      <c r="F2" s="109"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="34" t="s">
@@ -4681,11 +5583,138 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019DB3F1-EACB-C84B-A8AC-1AB7D29D4995}">
+  <dimension ref="B2:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="35"/>
+    <col min="2" max="2" width="13" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="111" t="s">
+        <v>322</v>
+      </c>
+      <c r="C2" s="35">
+        <v>0</v>
+      </c>
+      <c r="D2" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="E2" s="35">
+        <v>0.02</v>
+      </c>
+      <c r="F2" s="35">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G2" s="35">
+        <v>0.03</v>
+      </c>
+      <c r="H2" s="35">
+        <v>0.04</v>
+      </c>
+      <c r="I2" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="J2" s="35">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="111"/>
+      <c r="C3" s="35">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D3" s="35">
+        <v>0.08</v>
+      </c>
+      <c r="E3" s="47">
+        <v>0.09</v>
+      </c>
+      <c r="F3" s="47">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="H3" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="J3" s="35">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="111" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="47">
+        <v>0.05</v>
+      </c>
+      <c r="E4" s="47">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="47">
+        <v>0.25</v>
+      </c>
+      <c r="G4" s="47">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="111"/>
+      <c r="C5" s="47">
+        <v>0.75</v>
+      </c>
+      <c r="D5" s="47">
+        <v>1</v>
+      </c>
+      <c r="E5" s="47">
+        <v>1.5</v>
+      </c>
+      <c r="F5" s="47">
+        <v>2</v>
+      </c>
+      <c r="G5" s="47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="110"/>
+      <c r="C6" s="52"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="110"/>
+      <c r="C7" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B2:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A049609A-05AB-D543-9DD0-5AC0324048FB}">
   <dimension ref="B5:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B5" sqref="B5:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4742,12 +5771,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787C70AE-C051-1642-A6CB-97D2F568B5BC}">
   <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView zoomScale="136" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B9" sqref="B9:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4862,7 +5891,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAACC79-E576-FA47-9FAD-6537E6579EFB}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -5030,6 +6059,99 @@
       </c>
       <c r="D12" s="58" t="s">
         <v>275</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CF6425-97C2-6D4A-A83F-08A73FCBF017}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3">
+        <v>0.05</v>
+      </c>
+      <c r="D3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>365</v>
+      </c>
+      <c r="C4">
+        <v>0.75</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C5">
+        <v>0.1</v>
+      </c>
+      <c r="D5">
+        <v>0.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F23F0E-23F7-4D4A-A1CD-76A06C6C06B0}">
+  <dimension ref="C2:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -5534,6 +6656,1482 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C738158E-CC8D-5C4D-9772-76527F28A4B7}">
+  <dimension ref="B1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="89"/>
+    <col min="2" max="2" width="12.1640625" style="89" customWidth="1"/>
+    <col min="3" max="3" width="13" style="89" customWidth="1"/>
+    <col min="4" max="4" width="15" style="89" customWidth="1"/>
+    <col min="5" max="8" width="12.1640625" style="89" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="89"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" s="64" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="114"/>
+    </row>
+    <row r="3" spans="2:8" s="64" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="65" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>300</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>328</v>
+      </c>
+      <c r="G3" s="68" t="s">
+        <v>329</v>
+      </c>
+      <c r="H3" s="69" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" s="64" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="B4" s="70" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>302</v>
+      </c>
+      <c r="D4" s="72" t="s">
+        <v>325</v>
+      </c>
+      <c r="E4" s="73">
+        <v>99.67</v>
+      </c>
+      <c r="F4" s="74">
+        <v>99.42</v>
+      </c>
+      <c r="G4" s="71">
+        <v>99.5</v>
+      </c>
+      <c r="H4" s="75">
+        <v>99.13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" s="77" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="E5" s="79">
+        <v>99.68</v>
+      </c>
+      <c r="F5" s="80">
+        <v>99.43</v>
+      </c>
+      <c r="G5" s="81">
+        <v>99.5</v>
+      </c>
+      <c r="H5" s="82">
+        <v>99.13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" s="64" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="83" t="s">
+        <v>305</v>
+      </c>
+      <c r="C6" s="84" t="s">
+        <v>306</v>
+      </c>
+      <c r="D6" s="85" t="s">
+        <v>326</v>
+      </c>
+      <c r="E6" s="85">
+        <v>99.67</v>
+      </c>
+      <c r="F6" s="86">
+        <v>99.42</v>
+      </c>
+      <c r="G6" s="87">
+        <v>99.5</v>
+      </c>
+      <c r="H6" s="88">
+        <v>99.13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="89" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:8" s="64" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="112" t="s">
+        <v>308</v>
+      </c>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="114"/>
+    </row>
+    <row r="10" spans="2:8" s="64" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="65" t="s">
+        <v>324</v>
+      </c>
+      <c r="D10" s="66" t="s">
+        <v>300</v>
+      </c>
+      <c r="E10" s="66" t="s">
+        <v>327</v>
+      </c>
+      <c r="F10" s="67" t="s">
+        <v>328</v>
+      </c>
+      <c r="G10" s="68" t="s">
+        <v>329</v>
+      </c>
+      <c r="H10" s="69" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" s="64" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="B11" s="70" t="s">
+        <v>301</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>303</v>
+      </c>
+      <c r="D11" s="72" t="s">
+        <v>309</v>
+      </c>
+      <c r="E11" s="90">
+        <v>94.99</v>
+      </c>
+      <c r="F11" s="91">
+        <v>97.66</v>
+      </c>
+      <c r="G11" s="81">
+        <v>91.84</v>
+      </c>
+      <c r="H11" s="82">
+        <v>96.43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" s="77" t="s">
+        <v>310</v>
+      </c>
+      <c r="D12" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="E12" s="16">
+        <v>94.08</v>
+      </c>
+      <c r="F12" s="92">
+        <v>97.08</v>
+      </c>
+      <c r="G12" s="93" t="s">
+        <v>311</v>
+      </c>
+      <c r="H12" s="94">
+        <v>95.54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" s="64" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="83" t="s">
+        <v>305</v>
+      </c>
+      <c r="C13" s="84" t="s">
+        <v>312</v>
+      </c>
+      <c r="D13" s="85" t="s">
+        <v>313</v>
+      </c>
+      <c r="E13" s="85">
+        <v>92.98</v>
+      </c>
+      <c r="F13" s="86">
+        <v>96.79</v>
+      </c>
+      <c r="G13" s="71">
+        <v>91.84</v>
+      </c>
+      <c r="H13" s="75">
+        <v>96.43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:8" s="64" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="112" t="s">
+        <v>314</v>
+      </c>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="114"/>
+    </row>
+    <row r="16" spans="2:8" s="64" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="65" t="s">
+        <v>324</v>
+      </c>
+      <c r="D16" s="66" t="s">
+        <v>300</v>
+      </c>
+      <c r="E16" s="66" t="s">
+        <v>327</v>
+      </c>
+      <c r="F16" s="67" t="s">
+        <v>328</v>
+      </c>
+      <c r="G16" s="68" t="s">
+        <v>329</v>
+      </c>
+      <c r="H16" s="69" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" s="64" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="B17" s="70" t="s">
+        <v>301</v>
+      </c>
+      <c r="C17" s="71" t="s">
+        <v>315</v>
+      </c>
+      <c r="D17" s="72" t="s">
+        <v>316</v>
+      </c>
+      <c r="E17" s="73">
+        <v>12.91</v>
+      </c>
+      <c r="F17" s="74">
+        <v>78.11</v>
+      </c>
+      <c r="G17" s="71">
+        <v>53.35</v>
+      </c>
+      <c r="H17" s="75">
+        <v>72.48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="C18" s="77" t="s">
+        <v>317</v>
+      </c>
+      <c r="D18" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="E18" s="16">
+        <v>69.92</v>
+      </c>
+      <c r="F18" s="92">
+        <v>76.319999999999993</v>
+      </c>
+      <c r="G18" s="93" t="s">
+        <v>318</v>
+      </c>
+      <c r="H18" s="94">
+        <v>61.47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" s="64" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="83" t="s">
+        <v>305</v>
+      </c>
+      <c r="C19" s="84" t="s">
+        <v>319</v>
+      </c>
+      <c r="D19" s="85" t="s">
+        <v>320</v>
+      </c>
+      <c r="E19" s="85">
+        <v>64.67</v>
+      </c>
+      <c r="F19" s="95" t="s">
+        <v>321</v>
+      </c>
+      <c r="G19" s="84">
+        <v>65.63</v>
+      </c>
+      <c r="H19" s="88">
+        <v>66.97</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C15:H15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75A1BDA-DB0A-444D-8EAC-2B1EEF16EDCA}">
+  <dimension ref="B3:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C3" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="62">
+        <v>363</v>
+      </c>
+      <c r="D4" s="37">
+        <f>C4/$C$7</f>
+        <v>0.79955947136563876</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" s="62">
+        <v>33</v>
+      </c>
+      <c r="D5" s="37">
+        <f t="shared" ref="D5:D6" si="0">C5/$C$7</f>
+        <v>7.268722466960352E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" s="62">
+        <v>58</v>
+      </c>
+      <c r="D6" s="37">
+        <f t="shared" si="0"/>
+        <v>0.1277533039647577</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C7" s="62">
+        <f>SUM(C4:C6)</f>
+        <v>454</v>
+      </c>
+      <c r="D7" s="37">
+        <f>C7/$C$7</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F22595-EA40-0340-B09B-972358CE14DA}">
+  <dimension ref="D3:I20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D3" s="96"/>
+      <c r="E3" s="96" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" s="96" t="s">
+        <v>285</v>
+      </c>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D4" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="E4" s="55">
+        <v>363</v>
+      </c>
+      <c r="F4" s="99">
+        <v>273</v>
+      </c>
+      <c r="G4" s="102">
+        <f>F4/E4</f>
+        <v>0.75206611570247939</v>
+      </c>
+      <c r="H4" s="99">
+        <f>E4-F4</f>
+        <v>90</v>
+      </c>
+      <c r="I4" s="102">
+        <f>H4/E4</f>
+        <v>0.24793388429752067</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D5" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="E5" s="55">
+        <v>33</v>
+      </c>
+      <c r="F5" s="99">
+        <v>25</v>
+      </c>
+      <c r="G5" s="102">
+        <f t="shared" ref="G5:G6" si="0">F5/E5</f>
+        <v>0.75757575757575757</v>
+      </c>
+      <c r="H5" s="99">
+        <f t="shared" ref="H5:H6" si="1">E5-F5</f>
+        <v>8</v>
+      </c>
+      <c r="I5" s="102">
+        <f t="shared" ref="I5:I6" si="2">H5/E5</f>
+        <v>0.24242424242424243</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D6" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="E6" s="55">
+        <v>58</v>
+      </c>
+      <c r="F6" s="99">
+        <v>44</v>
+      </c>
+      <c r="G6" s="102">
+        <f t="shared" si="0"/>
+        <v>0.75862068965517238</v>
+      </c>
+      <c r="H6" s="99">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I6" s="102">
+        <f t="shared" si="2"/>
+        <v>0.2413793103448276</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="D7" s="98" t="s">
+        <v>336</v>
+      </c>
+      <c r="E7" s="100">
+        <f>E4/E6</f>
+        <v>6.2586206896551726</v>
+      </c>
+      <c r="F7" s="100">
+        <f t="shared" ref="F7:H7" si="3">F4/F6</f>
+        <v>6.2045454545454541</v>
+      </c>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100">
+        <f t="shared" si="3"/>
+        <v>6.4285714285714288</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="D8" s="98" t="s">
+        <v>335</v>
+      </c>
+      <c r="E8" s="101">
+        <f>E5/E6</f>
+        <v>0.56896551724137934</v>
+      </c>
+      <c r="F8" s="101">
+        <f t="shared" ref="F8:H8" si="4">F5/F6</f>
+        <v>0.56818181818181823</v>
+      </c>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101">
+        <f t="shared" si="4"/>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D15" s="96"/>
+      <c r="E15" s="96" t="s">
+        <v>233</v>
+      </c>
+      <c r="F15" s="96" t="s">
+        <v>285</v>
+      </c>
+      <c r="G15" s="96" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D16" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="E16" s="62" t="s">
+        <v>333</v>
+      </c>
+      <c r="F16" s="97" t="s">
+        <v>337</v>
+      </c>
+      <c r="G16" s="97" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D17" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="E17" s="62" t="s">
+        <v>334</v>
+      </c>
+      <c r="F17" s="97" t="s">
+        <v>338</v>
+      </c>
+      <c r="G17" s="97" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D18" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="E18" s="62" t="s">
+        <v>289</v>
+      </c>
+      <c r="F18" s="97" t="s">
+        <v>331</v>
+      </c>
+      <c r="G18" s="97" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="D19" s="98" t="s">
+        <v>336</v>
+      </c>
+      <c r="E19" s="97">
+        <v>6.3</v>
+      </c>
+      <c r="F19" s="97">
+        <v>6.2</v>
+      </c>
+      <c r="G19" s="97">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="D20" s="98" t="s">
+        <v>335</v>
+      </c>
+      <c r="E20" s="62">
+        <v>0.6</v>
+      </c>
+      <c r="F20" s="62">
+        <v>0.6</v>
+      </c>
+      <c r="G20" s="62">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE02438-7BEC-1A4B-A9D0-17EBA73CFC02}">
+  <dimension ref="B4:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="56" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="55">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="55">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>342</v>
+      </c>
+      <c r="D6" t="s">
+        <v>268</v>
+      </c>
+      <c r="E6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="55">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>344</v>
+      </c>
+      <c r="D7" t="s">
+        <v>262</v>
+      </c>
+      <c r="E7" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="55">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>346</v>
+      </c>
+      <c r="D8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="55">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>349</v>
+      </c>
+      <c r="D9" t="s">
+        <v>257</v>
+      </c>
+      <c r="E9" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="55">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>351</v>
+      </c>
+      <c r="D10" t="s">
+        <v>352</v>
+      </c>
+      <c r="E10" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="55">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E11" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="55">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>355</v>
+      </c>
+      <c r="D12" t="s">
+        <v>356</v>
+      </c>
+      <c r="E12" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="55">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>358</v>
+      </c>
+      <c r="D13" t="s">
+        <v>263</v>
+      </c>
+      <c r="E13" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="57">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>254</v>
+      </c>
+      <c r="D14" t="s">
+        <v>360</v>
+      </c>
+      <c r="E14" t="s">
+        <v>361</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0242ADB-AC69-1947-96C4-C2E0C80B530E}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="103"/>
+      <c r="B1" s="103" t="s">
+        <v>362</v>
+      </c>
+      <c r="C1" s="103" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="103" t="s">
+        <v>364</v>
+      </c>
+      <c r="B2" s="103">
+        <v>1</v>
+      </c>
+      <c r="C2" s="103">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="103" t="s">
+        <v>365</v>
+      </c>
+      <c r="B3" s="103">
+        <v>5</v>
+      </c>
+      <c r="C3" s="103">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="103" t="s">
+        <v>366</v>
+      </c>
+      <c r="B4" s="103">
+        <v>2</v>
+      </c>
+      <c r="C4" s="103">
+        <v>0.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A956B4-6D5B-2740-ABEA-A34EE433960D}">
+  <dimension ref="B3:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFE7814-DDAF-7143-B741-EB2317A2CB9A}">
+  <dimension ref="B1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="64"/>
+      <c r="C2" s="112" t="s">
+        <v>308</v>
+      </c>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="114"/>
+    </row>
+    <row r="3" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="64"/>
+      <c r="C3" s="65" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>300</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>328</v>
+      </c>
+      <c r="G3" s="68" t="s">
+        <v>329</v>
+      </c>
+      <c r="H3" s="69" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B4" s="70" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" s="72" t="s">
+        <v>367</v>
+      </c>
+      <c r="E4" s="104">
+        <v>94.99</v>
+      </c>
+      <c r="F4" s="105">
+        <v>97.66</v>
+      </c>
+      <c r="G4" s="106">
+        <v>91.84</v>
+      </c>
+      <c r="H4" s="107">
+        <v>96.43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" s="77" t="s">
+        <v>310</v>
+      </c>
+      <c r="D5" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="E5" s="16">
+        <v>94.08</v>
+      </c>
+      <c r="F5" s="92">
+        <v>97.08</v>
+      </c>
+      <c r="G5" s="93" t="s">
+        <v>311</v>
+      </c>
+      <c r="H5" s="94">
+        <v>95.54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="83" t="s">
+        <v>305</v>
+      </c>
+      <c r="C6" s="84" t="s">
+        <v>312</v>
+      </c>
+      <c r="D6" s="85" t="s">
+        <v>313</v>
+      </c>
+      <c r="E6" s="85">
+        <v>92.98</v>
+      </c>
+      <c r="F6" s="86">
+        <v>96.79</v>
+      </c>
+      <c r="G6" s="71">
+        <v>91.84</v>
+      </c>
+      <c r="H6" s="75">
+        <v>96.43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809BADF8-DCD8-AA4D-8591-AA233CE00153}">
+  <dimension ref="C2:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C3" s="103"/>
+      <c r="D3" s="115" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="115" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4" s="116" t="s">
+        <v>368</v>
+      </c>
+      <c r="D4" s="97">
+        <v>644</v>
+      </c>
+      <c r="E4" s="117">
+        <v>0.92700000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C5" s="116" t="s">
+        <v>281</v>
+      </c>
+      <c r="D5" s="97">
+        <v>51</v>
+      </c>
+      <c r="E5" s="117">
+        <v>7.2999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C6" s="116" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" s="97">
+        <f>SUM(D4:D5)</f>
+        <v>695</v>
+      </c>
+      <c r="E6" s="117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="103"/>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB633D2C-DD9C-104B-9D9D-0475372857CB}">
+  <dimension ref="D5:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D5" s="96"/>
+      <c r="E5" s="96" t="s">
+        <v>233</v>
+      </c>
+      <c r="F5" s="96" t="s">
+        <v>285</v>
+      </c>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D6" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="E6" s="55">
+        <v>644</v>
+      </c>
+      <c r="F6" s="99">
+        <v>483</v>
+      </c>
+      <c r="G6" s="102">
+        <f>F6/E6</f>
+        <v>0.75</v>
+      </c>
+      <c r="H6" s="99">
+        <f>E6-F6</f>
+        <v>161</v>
+      </c>
+      <c r="I6" s="102">
+        <f>H6/E6</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D7" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="E7" s="55">
+        <v>51</v>
+      </c>
+      <c r="F7" s="99">
+        <v>39</v>
+      </c>
+      <c r="G7" s="102">
+        <f>F7/E7</f>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="H7" s="99">
+        <f t="shared" ref="H7" si="0">E7-F7</f>
+        <v>12</v>
+      </c>
+      <c r="I7" s="102">
+        <f t="shared" ref="I7" si="1">H7/E7</f>
+        <v>0.23529411764705882</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="D8" s="98" t="s">
+        <v>290</v>
+      </c>
+      <c r="E8" s="100">
+        <f>E6/E7</f>
+        <v>12.627450980392156</v>
+      </c>
+      <c r="F8" s="100">
+        <f t="shared" ref="F8:H8" si="2">F6/F7</f>
+        <v>12.384615384615385</v>
+      </c>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100">
+        <f t="shared" si="2"/>
+        <v>13.416666666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D15" s="96"/>
+      <c r="E15" s="96" t="s">
+        <v>233</v>
+      </c>
+      <c r="F15" s="96" t="s">
+        <v>285</v>
+      </c>
+      <c r="G15" s="96" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D16" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>369</v>
+      </c>
+      <c r="F16" s="97" t="s">
+        <v>371</v>
+      </c>
+      <c r="G16" s="97" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D17" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>370</v>
+      </c>
+      <c r="F17" s="97" t="s">
+        <v>372</v>
+      </c>
+      <c r="G17" s="97" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="D18" s="98" t="s">
+        <v>290</v>
+      </c>
+      <c r="E18" s="97">
+        <v>12.6</v>
+      </c>
+      <c r="F18" s="97">
+        <v>12.4</v>
+      </c>
+      <c r="G18" s="63">
+        <v>13.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF0E40B-B96B-6F4F-8E6B-693729C259F4}">
+  <dimension ref="B3:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="56" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="55">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D4" t="s">
+        <v>376</v>
+      </c>
+      <c r="E4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="55">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5" t="s">
+        <v>379</v>
+      </c>
+      <c r="E5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="55">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>381</v>
+      </c>
+      <c r="D6" t="s">
+        <v>382</v>
+      </c>
+      <c r="E6" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="55">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>384</v>
+      </c>
+      <c r="D7" t="s">
+        <v>385</v>
+      </c>
+      <c r="E7" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="55">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>387</v>
+      </c>
+      <c r="D8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="55">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>390</v>
+      </c>
+      <c r="D9" t="s">
+        <v>391</v>
+      </c>
+      <c r="E9" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="55">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>393</v>
+      </c>
+      <c r="D10" t="s">
+        <v>394</v>
+      </c>
+      <c r="E10" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="55">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>394</v>
+      </c>
+      <c r="D11" t="s">
+        <v>396</v>
+      </c>
+      <c r="E11" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="55">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>398</v>
+      </c>
+      <c r="D12" t="s">
+        <v>399</v>
+      </c>
+      <c r="E12" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="57">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>401</v>
+      </c>
+      <c r="D13" t="s">
+        <v>402</v>
+      </c>
+      <c r="E13" t="s">
+        <v>403</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C6AF80-A29C-4664-8945-39173FEA3D6E}">
   <dimension ref="A4:K29"/>
@@ -6008,6 +8606,232 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C491CEAA-B4E5-F047-9D57-12CB0B49B3E2}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3">
+        <v>0.05</v>
+      </c>
+      <c r="D3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>365</v>
+      </c>
+      <c r="C4">
+        <v>0.05</v>
+      </c>
+      <c r="D4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C5">
+        <v>0.05</v>
+      </c>
+      <c r="D5">
+        <v>0.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF09184-1487-C445-8833-D6CA226ED2E8}">
+  <dimension ref="B3:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F56B19E-BE00-1B42-9F12-105EB61CEDCC}">
+  <dimension ref="B2:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="64"/>
+      <c r="C3" s="65" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>300</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>328</v>
+      </c>
+      <c r="G3" s="68" t="s">
+        <v>329</v>
+      </c>
+      <c r="H3" s="69" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B4" s="123" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" s="118" t="s">
+        <v>405</v>
+      </c>
+      <c r="D4" s="72" t="s">
+        <v>407</v>
+      </c>
+      <c r="E4" s="119">
+        <v>100</v>
+      </c>
+      <c r="F4" s="120">
+        <v>100</v>
+      </c>
+      <c r="G4" s="121">
+        <v>100</v>
+      </c>
+      <c r="H4" s="122">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B5" s="124"/>
+      <c r="C5" s="71" t="s">
+        <v>406</v>
+      </c>
+      <c r="D5" s="72" t="s">
+        <v>408</v>
+      </c>
+      <c r="E5" s="104">
+        <v>100</v>
+      </c>
+      <c r="F5" s="105">
+        <v>100</v>
+      </c>
+      <c r="G5" s="106">
+        <v>100</v>
+      </c>
+      <c r="H5" s="107">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" s="77" t="s">
+        <v>410</v>
+      </c>
+      <c r="D6" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="E6" s="16">
+        <v>100</v>
+      </c>
+      <c r="F6" s="92">
+        <v>100</v>
+      </c>
+      <c r="G6" s="93" t="s">
+        <v>404</v>
+      </c>
+      <c r="H6" s="94">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="83" t="s">
+        <v>305</v>
+      </c>
+      <c r="C7" s="84" t="s">
+        <v>406</v>
+      </c>
+      <c r="D7" s="85" t="s">
+        <v>409</v>
+      </c>
+      <c r="E7" s="85">
+        <v>100</v>
+      </c>
+      <c r="F7" s="86">
+        <v>100</v>
+      </c>
+      <c r="G7" s="71">
+        <v>100</v>
+      </c>
+      <c r="H7" s="75">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8601,7 +11425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BE78B5-187C-984C-BA57-F788A62E356E}">
   <dimension ref="B2:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:E5"/>
     </sheetView>
   </sheetViews>
@@ -8610,10 +11434,10 @@
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="108" t="s">
         <v>294</v>
       </c>
-      <c r="E2" s="63"/>
+      <c r="E2" s="108"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="55"/>
@@ -8626,7 +11450,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="108" t="s">
         <v>291</v>
       </c>
       <c r="C4" s="53" t="s">
@@ -8640,7 +11464,7 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="63"/>
+      <c r="B5" s="108"/>
       <c r="C5" s="53" t="s">
         <v>293</v>
       </c>

</xml_diff>

<commit_message>
añadir diagnóstico primario a tablas de CR
</commit_message>
<xml_diff>
--- a/documento/tablas/tablas_tfm.xlsx
+++ b/documento/tablas/tablas_tfm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Dropbox/Transporte_interno/Máster/Ciencia de Datos/TFM/documento/tablas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14770258-47D3-BA45-97CD-EB0397444F27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FF33AA-D4C8-CF4A-B958-967FD7EAB676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="4040" windowWidth="15880" windowHeight="13940" tabRatio="752" firstSheet="24" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="920" windowWidth="24420" windowHeight="17160" tabRatio="752" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Poblaciones estándar" sheetId="19" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="416">
   <si>
     <t>Grupo de edad</t>
   </si>
@@ -1307,6 +1307,21 @@
   </si>
   <si>
     <t>mRMR 4 genes</t>
+  </si>
+  <si>
+    <t>Caucásico</t>
+  </si>
+  <si>
+    <t>Afroamericano</t>
+  </si>
+  <si>
+    <t>Adenocarcinoma</t>
+  </si>
+  <si>
+    <t>Adenocarcinoma mucinoso</t>
+  </si>
+  <si>
+    <t>0,25</t>
   </si>
 </sst>
 </file>
@@ -1820,7 +1835,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2113,26 +2128,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2156,12 +2156,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -3199,7 +3227,7 @@
   <dimension ref="B2:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3482,8 +3510,8 @@
       <c r="H15" s="35"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="35" t="s">
-        <v>224</v>
+      <c r="B16" s="109" t="s">
+        <v>411</v>
       </c>
       <c r="C16" s="36">
         <v>212</v>
@@ -3493,7 +3521,7 @@
         <v>0.52475247524752477</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>224</v>
+        <v>411</v>
       </c>
       <c r="G16" s="35">
         <f t="shared" si="2"/>
@@ -3528,8 +3556,8 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="35" t="s">
-        <v>225</v>
+      <c r="B18" s="109" t="s">
+        <v>412</v>
       </c>
       <c r="C18" s="36">
         <v>19</v>
@@ -3539,7 +3567,7 @@
         <v>4.702970297029703E-2</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>225</v>
+        <v>412</v>
       </c>
       <c r="G18" s="35">
         <f t="shared" si="2"/>
@@ -3890,8 +3918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5CE535-076B-4A4A-931E-053042BF44D5}">
   <dimension ref="B1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:E47"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3906,14 +3934,14 @@
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="109" t="s">
+      <c r="C2" s="119" t="s">
         <v>229</v>
       </c>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109" t="s">
+      <c r="D2" s="119"/>
+      <c r="E2" s="119" t="s">
         <v>230</v>
       </c>
-      <c r="F2" s="109"/>
+      <c r="F2" s="119"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="34" t="s">
@@ -4526,10 +4554,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9964D0ED-D39A-9F40-BAAC-91509B1851FE}">
-  <dimension ref="B1:G33"/>
+  <dimension ref="B1:H37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F2" sqref="F2:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4642,7 +4670,7 @@
         <v>210</v>
       </c>
       <c r="G8" s="35" t="str">
-        <f t="shared" ref="G8:G20" si="1">C8 &amp; " (" &amp; ROUND(100*D8,1) &amp; "%)"</f>
+        <f t="shared" ref="G8:G14" si="1">C8 &amp; " (" &amp; ROUND(100*D8,1) &amp; "%)"</f>
         <v>16 (2,6%)</v>
       </c>
     </row>
@@ -4764,8 +4792,8 @@
       <c r="B15" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="F15" s="34" t="s">
-        <v>203</v>
+      <c r="F15" s="38" t="s">
+        <v>221</v>
       </c>
       <c r="G15" s="35"/>
     </row>
@@ -4781,14 +4809,14 @@
         <v>0.16935483870967741</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>204</v>
+        <v>411</v>
       </c>
       <c r="G16" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>105 (16,9%)</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+        <f>C30 &amp; " (" &amp; ROUND(100*D30,1) &amp; "%)"</f>
+        <v>293 (47,3%)</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="35" t="s">
         <v>206</v>
       </c>
@@ -4796,18 +4824,18 @@
         <v>225</v>
       </c>
       <c r="D17" s="37">
-        <f t="shared" ref="D17:D33" si="2">C17/$C$3</f>
+        <f t="shared" ref="D17:D37" si="2">C17/$C$3</f>
         <v>0.36290322580645162</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="G17" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>225 (36,3%)</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+        <f>C31 &amp; " (" &amp; ROUND(100*D31,1) &amp; "%)"</f>
+        <v>13 (2,1%)</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="35" t="s">
         <v>207</v>
       </c>
@@ -4819,14 +4847,14 @@
         <v>0.2870967741935484</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>207</v>
+        <v>412</v>
       </c>
       <c r="G18" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>178 (28,7%)</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+        <f>C32 &amp; " (" &amp; ROUND(100*D32,1) &amp; "%)"</f>
+        <v>65 (10,5%)</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="35" t="s">
         <v>205</v>
       </c>
@@ -4838,14 +4866,14 @@
         <v>0.1435483870967742</v>
       </c>
       <c r="F19" s="35" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="G19" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>89 (14,4%)</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+        <f>C33 &amp; " (" &amp; ROUND(100*D33,1) &amp; "%)"</f>
+        <v>248 (40%)</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="35" t="s">
         <v>208</v>
       </c>
@@ -4857,204 +4885,274 @@
         <v>3.7096774193548385E-2</v>
       </c>
       <c r="F20" s="43" t="s">
+        <v>222</v>
+      </c>
+      <c r="G20" s="43" t="str">
+        <f>C34 &amp; " (" &amp; ROUND(100*D34,1) &amp; "%)"</f>
+        <v>1 (0,2%)</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="128" t="s">
+        <v>240</v>
+      </c>
+      <c r="C21"/>
+      <c r="D21" s="37"/>
+      <c r="F21" s="128" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="127" t="s">
+        <v>413</v>
+      </c>
+      <c r="C22" s="108">
+        <v>517</v>
+      </c>
+      <c r="D22" s="37">
+        <f>C22/$C$3</f>
+        <v>0.83387096774193548</v>
+      </c>
+      <c r="F22" s="127" t="s">
+        <v>413</v>
+      </c>
+      <c r="G22" s="109" t="str">
+        <f>C22 &amp; " (" &amp; ROUND(100*D22,1) &amp; "%)"</f>
+        <v>517 (83,4%)</v>
+      </c>
+      <c r="H22" s="129"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="127" t="s">
+        <v>414</v>
+      </c>
+      <c r="C23" s="108">
+        <v>79</v>
+      </c>
+      <c r="D23" s="37">
+        <f t="shared" si="2"/>
+        <v>0.12741935483870967</v>
+      </c>
+      <c r="F23" s="127" t="s">
+        <v>414</v>
+      </c>
+      <c r="G23" s="109" t="str">
+        <f>C23 &amp; " (" &amp; ROUND(100*D23,1) &amp; "%)"</f>
+        <v>79 (12,7%)</v>
+      </c>
+      <c r="H23" s="129"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="127" t="s">
+        <v>243</v>
+      </c>
+      <c r="C24" s="108">
+        <v>24</v>
+      </c>
+      <c r="D24" s="37">
+        <f t="shared" si="2"/>
+        <v>3.870967741935484E-2</v>
+      </c>
+      <c r="F24" s="127" t="s">
+        <v>243</v>
+      </c>
+      <c r="G24" s="109" t="str">
+        <f>C24 &amp; " (" &amp; ROUND(100*D24,1) &amp; "%)"</f>
+        <v>24 (3,9%)</v>
+      </c>
+      <c r="H24" s="129"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="D25" s="37"/>
+      <c r="F25" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="G25" s="35"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="C26" s="40">
+        <v>5</v>
+      </c>
+      <c r="D26" s="37">
+        <f t="shared" si="2"/>
+        <v>8.0645161290322578E-3</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G26" s="35" t="str">
+        <f>C16 &amp; " (" &amp; ROUND(100*D16,1) &amp; "%)"</f>
+        <v>105 (16,9%)</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="C27" s="40">
+        <v>352</v>
+      </c>
+      <c r="D27" s="37">
+        <f t="shared" si="2"/>
+        <v>0.56774193548387097</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G27" s="35" t="str">
+        <f>C17 &amp; " (" &amp; ROUND(100*D17,1) &amp; "%)"</f>
+        <v>225 (36,3%)</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="G20" s="43" t="str">
-        <f t="shared" si="1"/>
+      <c r="C28" s="40">
+        <v>263</v>
+      </c>
+      <c r="D28" s="37">
+        <f t="shared" si="2"/>
+        <v>0.42419354838709677</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="G28" s="35" t="str">
+        <f>C18 &amp; " (" &amp; ROUND(100*D18,1) &amp; "%)"</f>
+        <v>178 (28,7%)</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="D29" s="37"/>
+      <c r="F29" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="G29" s="35" t="str">
+        <f>C19 &amp; " (" &amp; ROUND(100*D19,1) &amp; "%)"</f>
+        <v>89 (14,4%)</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="C30" s="40">
+        <v>293</v>
+      </c>
+      <c r="D30" s="37">
+        <f t="shared" si="2"/>
+        <v>0.47258064516129034</v>
+      </c>
+      <c r="F30" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="G30" s="43" t="str">
+        <f>C20 &amp; " (" &amp; ROUND(100*D20,1) &amp; "%)"</f>
         <v>23 (3,7%)</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="38" t="s">
-        <v>218</v>
-      </c>
-      <c r="D21" s="37"/>
-      <c r="F21" s="38" t="s">
-        <v>221</v>
-      </c>
-      <c r="G21" s="35"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="C22" s="40">
-        <v>5</v>
-      </c>
-      <c r="D22" s="37">
-        <f t="shared" si="2"/>
-        <v>8.0645161290322578E-3</v>
-      </c>
-      <c r="F22" s="35" t="s">
-        <v>224</v>
-      </c>
-      <c r="G22" s="35" t="str">
-        <f>C26 &amp; " (" &amp; ROUND(100*D26,1) &amp; "%)"</f>
-        <v>293 (47,3%)</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="C23" s="40">
-        <v>352</v>
-      </c>
-      <c r="D23" s="37">
-        <f t="shared" si="2"/>
-        <v>0.56774193548387097</v>
-      </c>
-      <c r="F23" s="35" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="G23" s="35" t="str">
-        <f>C27 &amp; " (" &amp; ROUND(100*D27,1) &amp; "%)"</f>
-        <v>13 (2,1%)</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="35" t="s">
+      <c r="C31" s="40">
+        <v>13</v>
+      </c>
+      <c r="D31" s="37">
+        <f t="shared" si="2"/>
+        <v>2.0967741935483872E-2</v>
+      </c>
+      <c r="F31" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="G31" s="35"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="C32" s="40">
+        <v>65</v>
+      </c>
+      <c r="D32" s="37">
+        <f t="shared" si="2"/>
+        <v>0.10483870967741936</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="G32" s="35" t="str">
+        <f>C36 &amp; " (" &amp; ROUND(100*D36,1) &amp; "%)"</f>
+        <v>491 (79,2%)</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="C24" s="40">
-        <v>263</v>
-      </c>
-      <c r="D24" s="37">
-        <f t="shared" si="2"/>
-        <v>0.42419354838709677</v>
-      </c>
-      <c r="F24" s="35" t="s">
-        <v>225</v>
-      </c>
-      <c r="G24" s="35" t="str">
-        <f>C28 &amp; " (" &amp; ROUND(100*D28,1) &amp; "%)"</f>
-        <v>65 (10,5%)</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="38" t="s">
-        <v>221</v>
-      </c>
-      <c r="D25" s="37"/>
-      <c r="F25" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="G25" s="35" t="str">
-        <f>C29 &amp; " (" &amp; ROUND(100*D29,1) &amp; "%)"</f>
-        <v>248 (40%)</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="35" t="s">
-        <v>224</v>
-      </c>
-      <c r="C26" s="40">
-        <v>293</v>
-      </c>
-      <c r="D26" s="37">
-        <f t="shared" si="2"/>
-        <v>0.47258064516129034</v>
-      </c>
-      <c r="F26" s="43" t="s">
+      <c r="C33" s="40">
+        <v>248</v>
+      </c>
+      <c r="D33" s="37">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="F33" s="43" t="s">
+        <v>228</v>
+      </c>
+      <c r="G33" s="43" t="str">
+        <f>C37 &amp; " (" &amp; ROUND(100*D37,1) &amp; "%)"</f>
+        <v>129 (20,8%)</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="G26" s="43" t="str">
-        <f>C30 &amp; " (" &amp; ROUND(100*D30,1) &amp; "%)"</f>
-        <v>1 (0,2%)</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="35" t="s">
-        <v>223</v>
-      </c>
-      <c r="C27" s="40">
-        <v>13</v>
-      </c>
-      <c r="D27" s="37">
-        <f t="shared" si="2"/>
-        <v>2.0967741935483872E-2</v>
-      </c>
-      <c r="F27" s="38" t="s">
+      <c r="C34" s="40">
+        <v>1</v>
+      </c>
+      <c r="D34" s="37">
+        <f t="shared" si="2"/>
+        <v>1.6129032258064516E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="G27" s="35"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="35" t="s">
-        <v>225</v>
-      </c>
-      <c r="C28" s="40">
-        <v>65</v>
-      </c>
-      <c r="D28" s="37">
-        <f t="shared" si="2"/>
-        <v>0.10483870967741936</v>
-      </c>
-      <c r="F28" s="35" t="s">
+      <c r="D35" s="37"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="G28" s="35" t="str">
-        <f>C32 &amp; " (" &amp; ROUND(100*D32,1) &amp; "%)"</f>
-        <v>491 (79,2%)</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="C29" s="40">
-        <v>248</v>
-      </c>
-      <c r="D29" s="37">
-        <f t="shared" si="2"/>
-        <v>0.4</v>
-      </c>
-      <c r="F29" s="43" t="s">
-        <v>228</v>
-      </c>
-      <c r="G29" s="43" t="str">
-        <f>C33 &amp; " (" &amp; ROUND(100*D33,1) &amp; "%)"</f>
-        <v>129 (20,8%)</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="35" t="s">
-        <v>222</v>
-      </c>
-      <c r="C30" s="40">
-        <v>1</v>
-      </c>
-      <c r="D30" s="37">
-        <f t="shared" si="2"/>
-        <v>1.6129032258064516E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="D31" s="37"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="35" t="s">
-        <v>227</v>
-      </c>
-      <c r="C32" s="40">
+      <c r="C36" s="40">
         <v>491</v>
       </c>
-      <c r="D32" s="37">
+      <c r="D36" s="37">
         <f t="shared" si="2"/>
         <v>0.79193548387096779</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="35" t="s">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="35" t="s">
         <v>234</v>
       </c>
-      <c r="C33" s="40">
+      <c r="C37" s="40">
         <v>129</v>
       </c>
-      <c r="D33" s="37">
+      <c r="D37" s="37">
         <f t="shared" si="2"/>
         <v>0.20806451612903226</v>
       </c>
@@ -5066,10 +5164,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEEA2B4-200E-DB41-881C-003B476C11AE}">
-  <dimension ref="B1:F38"/>
+  <dimension ref="B1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5084,14 +5182,14 @@
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="109" t="s">
+      <c r="C2" s="119" t="s">
         <v>229</v>
       </c>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109" t="s">
+      <c r="D2" s="119"/>
+      <c r="E2" s="119" t="s">
         <v>230</v>
       </c>
-      <c r="F2" s="109"/>
+      <c r="F2" s="119"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="34" t="s">
@@ -5349,229 +5447,346 @@
         <v>0.4606741573033708</v>
       </c>
     </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="C19" s="108"/>
+      <c r="D19" s="37"/>
+      <c r="F19" s="37"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="109" t="s">
+        <v>413</v>
+      </c>
+      <c r="C20" s="108">
+        <v>409</v>
+      </c>
+      <c r="D20" s="37">
+        <f t="shared" ref="D20:D22" si="2">C20/(C20+E20)</f>
+        <v>0.79110251450676983</v>
+      </c>
+      <c r="E20" s="108">
+        <v>108</v>
+      </c>
+      <c r="F20" s="37">
+        <f t="shared" ref="F20:F22" si="3">1-D20</f>
+        <v>0.20889748549323017</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="109" t="s">
+        <v>414</v>
+      </c>
+      <c r="C21" s="108">
+        <v>60</v>
+      </c>
+      <c r="D21" s="37">
+        <f t="shared" si="2"/>
+        <v>0.759493670886076</v>
+      </c>
+      <c r="E21" s="108">
+        <v>19</v>
+      </c>
+      <c r="F21" s="37">
+        <f t="shared" si="3"/>
+        <v>0.240506329113924</v>
+      </c>
+    </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="1"/>
-      <c r="C22" s="5" t="s">
+      <c r="B22" s="109" t="s">
+        <v>243</v>
+      </c>
+      <c r="C22" s="108">
+        <v>22</v>
+      </c>
+      <c r="D22" s="37">
+        <f t="shared" si="2"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E22" s="108">
+        <v>2</v>
+      </c>
+      <c r="F22" s="37">
+        <f t="shared" si="3"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+      <c r="C26" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="E22" s="46" t="s">
+      <c r="E26" s="46" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="34" t="s">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C27" s="5">
         <f>SUM(C5:C6)</f>
         <v>491</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D27" s="5">
         <f>SUM(E5:E6)</f>
         <v>129</v>
       </c>
-      <c r="E23" s="46"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="38" t="s">
+      <c r="E27" s="46"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="45" t="s">
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="45" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="47" t="s">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="C25" s="46" t="str">
+      <c r="C29" s="46" t="str">
         <f>C5 &amp; " (" &amp; ROUND(100*D5,1) &amp; "%)"</f>
         <v>260 (79%)</v>
       </c>
-      <c r="D25" s="46" t="str">
+      <c r="D29" s="46" t="str">
         <f>E5 &amp; " (" &amp; ROUND(100*F5,1) &amp; "%)"</f>
         <v>69 (21%)</v>
       </c>
-      <c r="E25" s="45"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="47" t="s">
+      <c r="E29" s="45"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="47" t="s">
         <v>217</v>
       </c>
-      <c r="C26" s="46" t="str">
+      <c r="C30" s="46" t="str">
         <f>C6 &amp; " (" &amp; ROUND(100*D6,1) &amp; "%)"</f>
         <v>231 (79,4%)</v>
       </c>
-      <c r="D26" s="46" t="str">
+      <c r="D30" s="46" t="str">
         <f>E6 &amp; " (" &amp; ROUND(100*F6,1) &amp; "%)"</f>
         <v>60 (20,6%)</v>
       </c>
-      <c r="E26" s="45"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="38" t="s">
+      <c r="E30" s="45"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="45" t="s">
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="45" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="47" t="s">
-        <v>210</v>
-      </c>
-      <c r="C28" s="46" t="str">
-        <f t="shared" ref="C28:C38" si="2">C8 &amp; " (" &amp; ROUND(100*D8,1) &amp; "%)"</f>
-        <v>14 (87,5%)</v>
-      </c>
-      <c r="D28" s="46" t="str">
-        <f t="shared" ref="D28:D33" si="3">E8 &amp; " (" &amp; ROUND(100*F8,1) &amp; "%)"</f>
-        <v>2 (12,5%)</v>
-      </c>
-      <c r="E28" s="45"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="47" t="s">
-        <v>211</v>
-      </c>
-      <c r="C29" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v>51 (86,4%)</v>
-      </c>
-      <c r="D29" s="46" t="str">
-        <f t="shared" si="3"/>
-        <v>8 (13,6%)</v>
-      </c>
-      <c r="E29" s="45"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="47" t="s">
-        <v>212</v>
-      </c>
-      <c r="C30" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v>85 (84,2%)</v>
-      </c>
-      <c r="D30" s="46" t="str">
-        <f t="shared" si="3"/>
-        <v>16 (15,8%)</v>
-      </c>
-      <c r="E30" s="45"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B31" s="47" t="s">
-        <v>213</v>
-      </c>
-      <c r="C31" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v>150 (86,7%)</v>
-      </c>
-      <c r="D31" s="46" t="str">
-        <f t="shared" si="3"/>
-        <v>23 (13,3%)</v>
-      </c>
-      <c r="E31" s="45"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" s="47" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C32" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v>120 (70,2%)</v>
+        <f t="shared" ref="C32:C42" si="4">C8 &amp; " (" &amp; ROUND(100*D8,1) &amp; "%)"</f>
+        <v>14 (87,5%)</v>
       </c>
       <c r="D32" s="46" t="str">
-        <f t="shared" si="3"/>
-        <v>51 (29,8%)</v>
+        <f t="shared" ref="D32:D37" si="5">E8 &amp; " (" &amp; ROUND(100*F8,1) &amp; "%)"</f>
+        <v>2 (12,5%)</v>
       </c>
       <c r="E32" s="45"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="47" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C33" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v>70 (71,4%)</v>
+        <f t="shared" si="4"/>
+        <v>51 (86,4%)</v>
       </c>
       <c r="D33" s="46" t="str">
-        <f t="shared" si="3"/>
-        <v>28 (28,6%)</v>
+        <f t="shared" si="5"/>
+        <v>8 (13,6%)</v>
       </c>
       <c r="E33" s="45"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="45" t="s">
-        <v>239</v>
-      </c>
+      <c r="B34" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="C34" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>85 (84,2%)</v>
+      </c>
+      <c r="D34" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v>16 (15,8%)</v>
+      </c>
+      <c r="E34" s="45"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="C35" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>150 (86,7%)</v>
+      </c>
+      <c r="D35" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v>23 (13,3%)</v>
+      </c>
+      <c r="E35" s="45"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="47" t="s">
+        <v>214</v>
+      </c>
+      <c r="C36" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>120 (70,2%)</v>
+      </c>
+      <c r="D36" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v>51 (29,8%)</v>
+      </c>
+      <c r="E36" s="45"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="C37" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>70 (71,4%)</v>
+      </c>
+      <c r="D37" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v>28 (28,6%)</v>
+      </c>
+      <c r="E37" s="45"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="45" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="47" t="s">
         <v>204</v>
       </c>
-      <c r="C35" s="46" t="str">
-        <f t="shared" si="2"/>
+      <c r="C39" s="46" t="str">
+        <f t="shared" si="4"/>
         <v>98 (93,3%)</v>
       </c>
-      <c r="D35" s="46" t="str">
+      <c r="D39" s="46" t="str">
         <f>E15 &amp; " (" &amp; ROUND(100*F15,1) &amp; "%)"</f>
         <v>7 (6,7%)</v>
       </c>
-      <c r="E35" s="45"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="47" t="s">
+      <c r="E39" s="45"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="47" t="s">
         <v>206</v>
       </c>
-      <c r="C36" s="46" t="str">
-        <f t="shared" si="2"/>
+      <c r="C40" s="46" t="str">
+        <f t="shared" si="4"/>
         <v>192 (85,3%)</v>
       </c>
-      <c r="D36" s="46" t="str">
+      <c r="D40" s="46" t="str">
         <f>E16 &amp; " (" &amp; ROUND(100*F16,1) &amp; "%)"</f>
         <v>33 (14,7%)</v>
       </c>
-      <c r="E36" s="45"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="47" t="s">
+      <c r="E40" s="45"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="47" t="s">
         <v>207</v>
       </c>
-      <c r="C37" s="46" t="str">
-        <f t="shared" si="2"/>
+      <c r="C41" s="46" t="str">
+        <f t="shared" si="4"/>
         <v>139 (78,1%)</v>
       </c>
-      <c r="D37" s="46" t="str">
+      <c r="D41" s="46" t="str">
         <f>E17 &amp; " (" &amp; ROUND(100*F17,1) &amp; "%)"</f>
         <v>39 (21,9%)</v>
       </c>
-      <c r="E37" s="45"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="47" t="s">
+      <c r="E41" s="45"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="47" t="s">
         <v>205</v>
       </c>
-      <c r="C38" s="46" t="str">
-        <f t="shared" si="2"/>
+      <c r="C42" s="46" t="str">
+        <f t="shared" si="4"/>
         <v>48 (53,9%)</v>
       </c>
-      <c r="D38" s="46" t="str">
+      <c r="D42" s="46" t="str">
         <f>E18 &amp; " (" &amp; ROUND(100*F18,1) &amp; "%)"</f>
         <v>41 (46,1%)</v>
       </c>
-      <c r="E38" s="45"/>
+      <c r="E42" s="45"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="C43" s="108"/>
+      <c r="D43" s="108"/>
+      <c r="E43" s="39" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="109" t="s">
+        <v>413</v>
+      </c>
+      <c r="C44" s="108" t="str">
+        <f>C20 &amp; " (" &amp; ROUND(100*D20,1) &amp; "%)"</f>
+        <v>409 (79,1%)</v>
+      </c>
+      <c r="D44" s="108" t="str">
+        <f>E20 &amp; " (" &amp; ROUND(100*F20,1) &amp; "%)"</f>
+        <v>108 (20,9%)</v>
+      </c>
+      <c r="E44" s="39"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="109" t="s">
+        <v>414</v>
+      </c>
+      <c r="C45" s="108" t="str">
+        <f t="shared" ref="C45:C46" si="6">C21 &amp; " (" &amp; ROUND(100*D21,1) &amp; "%)"</f>
+        <v>60 (75,9%)</v>
+      </c>
+      <c r="D45" s="108" t="str">
+        <f t="shared" ref="D45:D46" si="7">E21 &amp; " (" &amp; ROUND(100*F21,1) &amp; "%)"</f>
+        <v>19 (24,1%)</v>
+      </c>
+      <c r="E45" s="39"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="109" t="s">
+        <v>243</v>
+      </c>
+      <c r="C46" s="108" t="str">
+        <f t="shared" si="6"/>
+        <v>22 (91,7%)</v>
+      </c>
+      <c r="D46" s="108" t="str">
+        <f t="shared" si="7"/>
+        <v>2 (8,3%)</v>
+      </c>
+      <c r="E46" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5598,7 +5813,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="121" t="s">
         <v>322</v>
       </c>
       <c r="C2" s="35">
@@ -5627,7 +5842,7 @@
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="111"/>
+      <c r="B3" s="121"/>
       <c r="C3" s="35">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -5654,7 +5869,7 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="121" t="s">
         <v>323</v>
       </c>
       <c r="C4" s="35">
@@ -5674,7 +5889,7 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="111"/>
+      <c r="B5" s="121"/>
       <c r="C5" s="47">
         <v>0.75</v>
       </c>
@@ -5692,11 +5907,11 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="110"/>
+      <c r="B6" s="120"/>
       <c r="C6" s="52"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="110"/>
+      <c r="B7" s="120"/>
       <c r="C7" s="52"/>
     </row>
   </sheetData>
@@ -6676,14 +6891,14 @@
   <sheetData>
     <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" s="64" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="112" t="s">
+      <c r="C2" s="122" t="s">
         <v>299</v>
       </c>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="114"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="124"/>
     </row>
     <row r="3" spans="2:8" s="64" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="65" t="s">
@@ -6781,14 +6996,14 @@
     </row>
     <row r="8" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:8" s="64" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="112" t="s">
+      <c r="C9" s="122" t="s">
         <v>308</v>
       </c>
-      <c r="D9" s="113"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="113"/>
-      <c r="G9" s="113"/>
-      <c r="H9" s="114"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="124"/>
     </row>
     <row r="10" spans="2:8" s="64" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="65" t="s">
@@ -6881,14 +7096,14 @@
     </row>
     <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:8" s="64" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="112" t="s">
+      <c r="C15" s="122" t="s">
         <v>314</v>
       </c>
-      <c r="D15" s="113"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="113"/>
-      <c r="G15" s="113"/>
-      <c r="H15" s="114"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="124"/>
     </row>
     <row r="16" spans="2:8" s="64" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C16" s="65" t="s">
@@ -7595,14 +7810,14 @@
     <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="64"/>
-      <c r="C2" s="112" t="s">
+      <c r="C2" s="122" t="s">
         <v>308</v>
       </c>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="114"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="124"/>
     </row>
     <row r="3" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="64"/>
@@ -7722,44 +7937,44 @@
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C3" s="103"/>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="115" t="s">
+      <c r="E3" s="110" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C4" s="116" t="s">
+      <c r="C4" s="111" t="s">
         <v>368</v>
       </c>
       <c r="D4" s="97">
         <v>644</v>
       </c>
-      <c r="E4" s="117">
+      <c r="E4" s="112">
         <v>0.92700000000000005</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C5" s="116" t="s">
+      <c r="C5" s="111" t="s">
         <v>281</v>
       </c>
       <c r="D5" s="97">
         <v>51</v>
       </c>
-      <c r="E5" s="117">
+      <c r="E5" s="112">
         <v>7.2999999999999995E-2</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C6" s="116" t="s">
+      <c r="C6" s="111" t="s">
         <v>233</v>
       </c>
       <c r="D6" s="97">
         <f>SUM(D4:D5)</f>
         <v>695</v>
       </c>
-      <c r="E6" s="117">
+      <c r="E6" s="112">
         <v>1</v>
       </c>
     </row>
@@ -7850,7 +8065,7 @@
         <v>0.23529411764705882</v>
       </c>
     </row>
-    <row r="8" spans="4:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:9" ht="34" x14ac:dyDescent="0.2">
       <c r="D8" s="98" t="s">
         <v>290</v>
       </c>
@@ -8707,7 +8922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F56B19E-BE00-1B42-9F12-105EB61CEDCC}">
   <dimension ref="B2:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -8717,7 +8932,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="64"/>
       <c r="C3" s="65" t="s">
         <v>324</v>
@@ -8739,30 +8954,30 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="B4" s="123" t="s">
+      <c r="B4" s="125" t="s">
         <v>301</v>
       </c>
-      <c r="C4" s="118" t="s">
+      <c r="C4" s="113" t="s">
         <v>405</v>
       </c>
       <c r="D4" s="72" t="s">
         <v>407</v>
       </c>
-      <c r="E4" s="119">
+      <c r="E4" s="114">
         <v>100</v>
       </c>
-      <c r="F4" s="120">
+      <c r="F4" s="115">
         <v>100</v>
       </c>
-      <c r="G4" s="121">
+      <c r="G4" s="116">
         <v>100</v>
       </c>
-      <c r="H4" s="122">
+      <c r="H4" s="117">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="B5" s="124"/>
+      <c r="B5" s="126"/>
       <c r="C5" s="71" t="s">
         <v>406</v>
       </c>
@@ -11434,10 +11649,10 @@
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
-      <c r="D2" s="108" t="s">
+      <c r="D2" s="118" t="s">
         <v>294</v>
       </c>
-      <c r="E2" s="108"/>
+      <c r="E2" s="118"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="55"/>
@@ -11450,7 +11665,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="118" t="s">
         <v>291</v>
       </c>
       <c r="C4" s="53" t="s">
@@ -11464,7 +11679,7 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="108"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="53" t="s">
         <v>293</v>
       </c>

</xml_diff>

<commit_message>
añadir conclusiones capítulo 4
</commit_message>
<xml_diff>
--- a/documento/tablas/tablas_tfm.xlsx
+++ b/documento/tablas/tablas_tfm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Dropbox/Transporte_interno/Máster/Ciencia de Datos/TFM/documento/tablas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FF33AA-D4C8-CF4A-B958-967FD7EAB676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7723E2D-4B06-1B4F-BE4A-53B73DB0F575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="920" windowWidth="24420" windowHeight="17160" tabRatio="752" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="480" windowWidth="25740" windowHeight="20540" tabRatio="752" firstSheet="27" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Poblaciones estándar" sheetId="19" r:id="rId1"/>
@@ -45,6 +45,12 @@
     <sheet name="29 - tuningSVM CRB" sheetId="51" r:id="rId30"/>
     <sheet name="30 - tuningkNN CRB" sheetId="52" r:id="rId31"/>
     <sheet name="31 - mejores modelos CRB" sheetId="53" r:id="rId32"/>
+    <sheet name="32 - tipo de muestra CRM" sheetId="54" r:id="rId33"/>
+    <sheet name="33 - traintest CRM" sheetId="55" r:id="rId34"/>
+    <sheet name="34 - genes CRM" sheetId="56" r:id="rId35"/>
+    <sheet name="35 - tuningSVM CRM" sheetId="57" r:id="rId36"/>
+    <sheet name="36 - tuningkNN CRM" sheetId="58" r:id="rId37"/>
+    <sheet name="37 - mejores modelos CRM" sheetId="59" r:id="rId38"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="486">
   <si>
     <t>Grupo de edad</t>
   </si>
@@ -1322,6 +1328,220 @@
   </si>
   <si>
     <t>0,25</t>
+  </si>
+  <si>
+    <t>Tejido normal</t>
+  </si>
+  <si>
+    <t>Adenocarcinoma
+mucinoso</t>
+  </si>
+  <si>
+    <t>530 (100%)</t>
+  </si>
+  <si>
+    <t>87 (100%)</t>
+  </si>
+  <si>
+    <t>398 (75,1%)</t>
+  </si>
+  <si>
+    <t>66 (75,9%)</t>
+  </si>
+  <si>
+    <t>132 (24,9%)</t>
+  </si>
+  <si>
+    <t>21 (24,1%)</t>
+  </si>
+  <si>
+    <t>Proporción
+adenoc./sanos</t>
+  </si>
+  <si>
+    <t>Proporción
+adenoc. muc./sanos</t>
+  </si>
+  <si>
+    <t>GTF2IRD1</t>
+  </si>
+  <si>
+    <t>CD79B</t>
+  </si>
+  <si>
+    <t>SCN4A</t>
+  </si>
+  <si>
+    <t>MUC2</t>
+  </si>
+  <si>
+    <t>BTK</t>
+  </si>
+  <si>
+    <t>CLEC3B</t>
+  </si>
+  <si>
+    <t>CSE1L</t>
+  </si>
+  <si>
+    <t>BRCA1</t>
+  </si>
+  <si>
+    <t>SCGN</t>
+  </si>
+  <si>
+    <t>FAS</t>
+  </si>
+  <si>
+    <t>SLC11A1</t>
+  </si>
+  <si>
+    <t>OSBPL3</t>
+  </si>
+  <si>
+    <t>PVT1</t>
+  </si>
+  <si>
+    <t>GDPD5</t>
+  </si>
+  <si>
+    <t>CPNE7</t>
+  </si>
+  <si>
+    <t>CDH3</t>
+  </si>
+  <si>
+    <t>ATP2B3</t>
+  </si>
+  <si>
+    <t>79,28</t>
+  </si>
+  <si>
+    <t>mRMR 9 genes</t>
+  </si>
+  <si>
+    <t>$c$ = 5
+$\gamma$ = 0,07</t>
+  </si>
+  <si>
+    <t>No hay relación</t>
+  </si>
+  <si>
+    <t>UK Biobank</t>
+  </si>
+  <si>
+    <t>Relación con otros cánceres</t>
+  </si>
+  <si>
+    <t>Relación con consumo de alcohol</t>
+  </si>
+  <si>
+    <t>Fuentes</t>
+  </si>
+  <si>
+    <t>http://europepmc.org/article/MED/29059683</t>
+  </si>
+  <si>
+    <t>http://europepmc.org/article/MED/26098869</t>
+  </si>
+  <si>
+    <t>http://europepmc.org/article/MED/24163127</t>
+  </si>
+  <si>
+    <t>http://europepmc.org/article/MED/20972438</t>
+  </si>
+  <si>
+    <t>http://europepmc.org/article/MED/29058716</t>
+  </si>
+  <si>
+    <t>http://europepmc.org/article/MED/27911795</t>
+  </si>
+  <si>
+    <t>http://europepmc.org/article/MED/30643251</t>
+  </si>
+  <si>
+    <t>http://europepmc.org/article/MED/25751625</t>
+  </si>
+  <si>
+    <t>Relación con otros cánceres; consumo de alcohol</t>
+  </si>
+  <si>
+    <t>Liver</t>
+  </si>
+  <si>
+    <t>Cirrhosis</t>
+  </si>
+  <si>
+    <t>smoking</t>
+  </si>
+  <si>
+    <t>alcohol</t>
+  </si>
+  <si>
+    <t>diabetes tipo ii</t>
+  </si>
+  <si>
+    <t>Edad de iniciación a fumar PMID: 30643251</t>
+  </si>
+  <si>
+    <t>cancer</t>
+  </si>
+  <si>
+    <t>alcohol 27911795</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fumar PMID: </t>
+  </si>
+  <si>
+    <t>colon</t>
+  </si>
+  <si>
+    <t>rectum</t>
+  </si>
+  <si>
+    <t>overweight</t>
+  </si>
+  <si>
+    <t>smok</t>
+  </si>
+  <si>
+    <t>diabetes</t>
+  </si>
+  <si>
+    <t>bowel</t>
+  </si>
+  <si>
+    <t>Crohn</t>
+  </si>
+  <si>
+    <t>colitis</t>
+  </si>
+  <si>
+    <t>10.1007/BF00121166</t>
+  </si>
+  <si>
+    <t>30679032, 30643251</t>
+  </si>
+  <si>
+    <t>cáncer de cérvix 30412241</t>
+  </si>
+  <si>
+    <t>mrmrm</t>
+  </si>
+  <si>
+    <t>(ver arriba)</t>
+  </si>
+  <si>
+    <t>Biobank</t>
+  </si>
+  <si>
+    <t>mama 29059683 y próstata 29892016</t>
+  </si>
+  <si>
+    <t>cáncer de pulmón 26732429 de piel (Biobank)</t>
+  </si>
+  <si>
+    <t>﻿Liu2019</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1552,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1426,8 +1646,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF494949"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1437,6 +1663,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1829,13 +2061,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2156,6 +2389,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2183,16 +2432,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="4" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
@@ -3934,14 +4182,14 @@
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="125" t="s">
         <v>229</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119" t="s">
+      <c r="D2" s="125"/>
+      <c r="E2" s="125" t="s">
         <v>230</v>
       </c>
-      <c r="F2" s="119"/>
+      <c r="F2" s="125"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="34" t="s">
@@ -4893,17 +5141,17 @@
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="128" t="s">
+      <c r="B21" s="120" t="s">
         <v>240</v>
       </c>
       <c r="C21"/>
       <c r="D21" s="37"/>
-      <c r="F21" s="128" t="s">
+      <c r="F21" s="120" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="127" t="s">
+      <c r="B22" s="119" t="s">
         <v>413</v>
       </c>
       <c r="C22" s="108">
@@ -4913,17 +5161,17 @@
         <f>C22/$C$3</f>
         <v>0.83387096774193548</v>
       </c>
-      <c r="F22" s="127" t="s">
+      <c r="F22" s="119" t="s">
         <v>413</v>
       </c>
       <c r="G22" s="109" t="str">
         <f>C22 &amp; " (" &amp; ROUND(100*D22,1) &amp; "%)"</f>
         <v>517 (83,4%)</v>
       </c>
-      <c r="H22" s="129"/>
+      <c r="H22" s="121"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="127" t="s">
+      <c r="B23" s="119" t="s">
         <v>414</v>
       </c>
       <c r="C23" s="108">
@@ -4933,17 +5181,17 @@
         <f t="shared" si="2"/>
         <v>0.12741935483870967</v>
       </c>
-      <c r="F23" s="127" t="s">
+      <c r="F23" s="119" t="s">
         <v>414</v>
       </c>
       <c r="G23" s="109" t="str">
         <f>C23 &amp; " (" &amp; ROUND(100*D23,1) &amp; "%)"</f>
         <v>79 (12,7%)</v>
       </c>
-      <c r="H23" s="129"/>
+      <c r="H23" s="121"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="127" t="s">
+      <c r="B24" s="119" t="s">
         <v>243</v>
       </c>
       <c r="C24" s="108">
@@ -4953,14 +5201,14 @@
         <f t="shared" si="2"/>
         <v>3.870967741935484E-2</v>
       </c>
-      <c r="F24" s="127" t="s">
+      <c r="F24" s="119" t="s">
         <v>243</v>
       </c>
       <c r="G24" s="109" t="str">
         <f>C24 &amp; " (" &amp; ROUND(100*D24,1) &amp; "%)"</f>
         <v>24 (3,9%)</v>
       </c>
-      <c r="H24" s="129"/>
+      <c r="H24" s="121"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="38" t="s">
@@ -5166,7 +5414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEEA2B4-200E-DB41-881C-003B476C11AE}">
   <dimension ref="B1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B44" sqref="B44:B46"/>
     </sheetView>
   </sheetViews>
@@ -5182,14 +5430,14 @@
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="125" t="s">
         <v>229</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119" t="s">
+      <c r="D2" s="125"/>
+      <c r="E2" s="125" t="s">
         <v>230</v>
       </c>
-      <c r="F2" s="119"/>
+      <c r="F2" s="125"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="34" t="s">
@@ -5813,7 +6061,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="127" t="s">
         <v>322</v>
       </c>
       <c r="C2" s="35">
@@ -5842,7 +6090,7 @@
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="121"/>
+      <c r="B3" s="127"/>
       <c r="C3" s="35">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -5869,7 +6117,7 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="127" t="s">
         <v>323</v>
       </c>
       <c r="C4" s="35">
@@ -5889,7 +6137,7 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="121"/>
+      <c r="B5" s="127"/>
       <c r="C5" s="47">
         <v>0.75</v>
       </c>
@@ -5907,11 +6155,11 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="120"/>
+      <c r="B6" s="126"/>
       <c r="C6" s="52"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="120"/>
+      <c r="B7" s="126"/>
       <c r="C7" s="52"/>
     </row>
   </sheetData>
@@ -6108,13 +6356,17 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAACC79-E576-FA47-9FAD-6537E6579EFB}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D12"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="26.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="41"/>
@@ -6140,10 +6392,10 @@
       <c r="A3" s="55">
         <v>1</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="133" t="s">
         <v>249</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="133" t="s">
         <v>249</v>
       </c>
       <c r="D3" s="49" t="s">
@@ -6154,10 +6406,10 @@
       <c r="A4" s="55">
         <v>2</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="133" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="133" t="s">
         <v>252</v>
       </c>
       <c r="D4" s="49" t="s">
@@ -6168,10 +6420,10 @@
       <c r="A5" s="55">
         <v>3</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="133" t="s">
         <v>254</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="133" t="s">
         <v>254</v>
       </c>
       <c r="D5" s="49" t="s">
@@ -6182,10 +6434,10 @@
       <c r="A6" s="55">
         <v>4</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="133" t="s">
         <v>256</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="133" t="s">
         <v>257</v>
       </c>
       <c r="D6" s="49" t="s">
@@ -6196,7 +6448,7 @@
       <c r="A7" s="55">
         <v>5</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="133" t="s">
         <v>259</v>
       </c>
       <c r="C7" s="49" t="s">
@@ -6210,7 +6462,7 @@
       <c r="A8" s="55">
         <v>6</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="133" t="s">
         <v>262</v>
       </c>
       <c r="C8" s="49" t="s">
@@ -6224,7 +6476,7 @@
       <c r="A9" s="55">
         <v>7</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="133" t="s">
         <v>265</v>
       </c>
       <c r="C9" s="49" t="s">
@@ -6276,7 +6528,124 @@
         <v>275</v>
       </c>
     </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="133" t="s">
+        <v>249</v>
+      </c>
+      <c r="C20" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="133" t="s">
+        <v>251</v>
+      </c>
+      <c r="C21" t="s">
+        <v>448</v>
+      </c>
+      <c r="D21" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="133" t="s">
+        <v>254</v>
+      </c>
+      <c r="C22" t="s">
+        <v>448</v>
+      </c>
+      <c r="D22" s="134" t="s">
+        <v>451</v>
+      </c>
+      <c r="E22" s="134" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="133" t="s">
+        <v>256</v>
+      </c>
+      <c r="C23" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="133" t="s">
+        <v>259</v>
+      </c>
+      <c r="C24" t="s">
+        <v>448</v>
+      </c>
+      <c r="D24" s="134" t="s">
+        <v>453</v>
+      </c>
+      <c r="E24" t="s">
+        <v>454</v>
+      </c>
+      <c r="G24" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="133" t="s">
+        <v>262</v>
+      </c>
+      <c r="C25" t="s">
+        <v>449</v>
+      </c>
+      <c r="D25" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="133" t="s">
+        <v>265</v>
+      </c>
+      <c r="C26" t="s">
+        <v>449</v>
+      </c>
+      <c r="D26" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="133" t="s">
+        <v>252</v>
+      </c>
+      <c r="C27" t="s">
+        <v>459</v>
+      </c>
+      <c r="D27" s="134" t="s">
+        <v>451</v>
+      </c>
+      <c r="E27" s="134" t="s">
+        <v>458</v>
+      </c>
+      <c r="F27" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="133" t="s">
+        <v>257</v>
+      </c>
+      <c r="C28" t="s">
+        <v>446</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D22" r:id="rId1" xr:uid="{32442C13-8085-BE4F-B46F-15A8AF37E95F}"/>
+    <hyperlink ref="E22" r:id="rId2" xr:uid="{CCC9D002-2B2C-6542-87C4-BD93964CA31A}"/>
+    <hyperlink ref="D24" r:id="rId3" xr:uid="{B18EABC3-2E56-C947-BFD6-F32EAB436A0B}"/>
+    <hyperlink ref="D27" r:id="rId4" xr:uid="{A5D4DC61-A453-5444-9224-16D427E0510F}"/>
+    <hyperlink ref="E27" r:id="rId5" xr:uid="{1E9B5A15-EBE2-D741-9CBA-18AA9E091BD7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6891,14 +7260,14 @@
   <sheetData>
     <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" s="64" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="122" t="s">
+      <c r="C2" s="128" t="s">
         <v>299</v>
       </c>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="124"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="130"/>
     </row>
     <row r="3" spans="2:8" s="64" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="65" t="s">
@@ -6996,14 +7365,14 @@
     </row>
     <row r="8" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:8" s="64" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="122" t="s">
+      <c r="C9" s="128" t="s">
         <v>308</v>
       </c>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="124"/>
+      <c r="D9" s="129"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="129"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="130"/>
     </row>
     <row r="10" spans="2:8" s="64" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="65" t="s">
@@ -7096,14 +7465,14 @@
     </row>
     <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:8" s="64" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="122" t="s">
+      <c r="C15" s="128" t="s">
         <v>314</v>
       </c>
-      <c r="D15" s="123"/>
-      <c r="E15" s="123"/>
-      <c r="F15" s="123"/>
-      <c r="G15" s="123"/>
-      <c r="H15" s="124"/>
+      <c r="D15" s="129"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="129"/>
+      <c r="G15" s="129"/>
+      <c r="H15" s="130"/>
     </row>
     <row r="16" spans="2:8" s="64" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C16" s="65" t="s">
@@ -7284,7 +7653,7 @@
   <dimension ref="D3:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:J23"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7536,10 +7905,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE02438-7BEC-1A4B-A9D0-17EBA73CFC02}">
-  <dimension ref="B4:E14"/>
+  <dimension ref="B4:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7696,6 +8065,70 @@
       </c>
       <c r="E14" t="s">
         <v>361</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>460</v>
+      </c>
+      <c r="D18" t="s">
+        <v>466</v>
+      </c>
+      <c r="E18" t="s">
+        <v>461</v>
+      </c>
+      <c r="F18" t="s">
+        <v>462</v>
+      </c>
+      <c r="G18" t="s">
+        <v>463</v>
+      </c>
+      <c r="H18" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>344</v>
+      </c>
+      <c r="F21" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>351</v>
+      </c>
+      <c r="F24" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>262</v>
+      </c>
+      <c r="G25" t="s">
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -7802,7 +8235,7 @@
   <dimension ref="B1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7810,14 +8243,14 @@
     <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="64"/>
-      <c r="C2" s="122" t="s">
+      <c r="C2" s="128" t="s">
         <v>308</v>
       </c>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="124"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="130"/>
     </row>
     <row r="3" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="64"/>
@@ -7922,7 +8355,7 @@
   <dimension ref="C2:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7998,7 +8431,7 @@
   <dimension ref="D5:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:G18"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8180,15 +8613,23 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF0E40B-B96B-6F4F-8E6B-693729C259F4}">
-  <dimension ref="B3:E13"/>
+  <dimension ref="A3:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E13"/>
+      <selection activeCell="C16" sqref="C16:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="5" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="6" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="56" t="s">
         <v>279</v>
       </c>
@@ -8202,7 +8643,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="55">
         <v>1</v>
       </c>
@@ -8216,7 +8657,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="55">
         <v>2</v>
       </c>
@@ -8230,7 +8671,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="55">
         <v>3</v>
       </c>
@@ -8244,7 +8685,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="55">
         <v>4</v>
       </c>
@@ -8258,7 +8699,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="55">
         <v>5</v>
       </c>
@@ -8272,7 +8713,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="55">
         <v>6</v>
       </c>
@@ -8286,7 +8727,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="55">
         <v>7</v>
       </c>
@@ -8300,7 +8741,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="55">
         <v>8</v>
       </c>
@@ -8314,7 +8755,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="55">
         <v>9</v>
       </c>
@@ -8328,7 +8769,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="57">
         <v>10</v>
       </c>
@@ -8342,7 +8783,152 @@
         <v>403</v>
       </c>
     </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>469</v>
+      </c>
+      <c r="D16" t="s">
+        <v>470</v>
+      </c>
+      <c r="E16" t="s">
+        <v>466</v>
+      </c>
+      <c r="F16" t="s">
+        <v>471</v>
+      </c>
+      <c r="G16" t="s">
+        <v>472</v>
+      </c>
+      <c r="H16" t="s">
+        <v>463</v>
+      </c>
+      <c r="I16" t="s">
+        <v>473</v>
+      </c>
+      <c r="J16" t="s">
+        <v>474</v>
+      </c>
+      <c r="K16" t="s">
+        <v>475</v>
+      </c>
+      <c r="L16" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>364</v>
+      </c>
+      <c r="B17" t="s">
+        <v>375</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>378</v>
+      </c>
+      <c r="C18" s="134" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>381</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>384</v>
+      </c>
+      <c r="H20" s="135" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>365</v>
+      </c>
+      <c r="B22" t="s">
+        <v>376</v>
+      </c>
+      <c r="C22" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>382</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C18" r:id="rId1" display="https://doi.org/10.1007/BF00121166" xr:uid="{55B317CA-7CDC-1743-9B51-EF062373CBD7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8830,7 +9416,7 @@
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8886,7 +9472,7 @@
   <dimension ref="B3:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8954,7 +9540,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="B4" s="125" t="s">
+      <c r="B4" s="131" t="s">
         <v>301</v>
       </c>
       <c r="C4" s="113" t="s">
@@ -8977,7 +9563,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="B5" s="126"/>
+      <c r="B5" s="132"/>
       <c r="C5" s="71" t="s">
         <v>406</v>
       </c>
@@ -9047,6 +9633,842 @@
   <mergeCells count="1">
     <mergeCell ref="B4:B5"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC3E755-F734-BD4B-A6B4-444810D2445C}">
+  <dimension ref="C2:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="103"/>
+      <c r="D3" s="110" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="110" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="111" t="s">
+        <v>413</v>
+      </c>
+      <c r="D4" s="97">
+        <v>530</v>
+      </c>
+      <c r="E4" s="112">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="G4" s="121"/>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" s="111" t="s">
+        <v>414</v>
+      </c>
+      <c r="D5" s="97">
+        <v>87</v>
+      </c>
+      <c r="E5" s="112">
+        <v>0.13</v>
+      </c>
+      <c r="G5" s="121"/>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="111" t="s">
+        <v>416</v>
+      </c>
+      <c r="D6" s="97">
+        <v>51</v>
+      </c>
+      <c r="E6" s="112">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G6" s="121"/>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="111" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" s="97">
+        <f>SUM(D4:D6)</f>
+        <v>668</v>
+      </c>
+      <c r="E7" s="112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1645F2B9-003E-5A4E-87A8-53335CFC6873}">
+  <dimension ref="D3:I20"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G20" sqref="D15:G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D3" s="96"/>
+      <c r="E3" s="96" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" s="96" t="s">
+        <v>285</v>
+      </c>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D4" s="34" t="s">
+        <v>413</v>
+      </c>
+      <c r="E4" s="55">
+        <v>530</v>
+      </c>
+      <c r="F4" s="99">
+        <v>398</v>
+      </c>
+      <c r="G4" s="102">
+        <f>F4/E4</f>
+        <v>0.75094339622641515</v>
+      </c>
+      <c r="H4" s="99">
+        <f>E4-F4</f>
+        <v>132</v>
+      </c>
+      <c r="I4" s="102">
+        <f>H4/E4</f>
+        <v>0.24905660377358491</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="D5" s="122" t="s">
+        <v>417</v>
+      </c>
+      <c r="E5" s="55">
+        <v>87</v>
+      </c>
+      <c r="F5" s="99">
+        <v>66</v>
+      </c>
+      <c r="G5" s="102">
+        <f t="shared" ref="G5:G6" si="0">F5/E5</f>
+        <v>0.75862068965517238</v>
+      </c>
+      <c r="H5" s="99">
+        <f t="shared" ref="H5:H6" si="1">E5-F5</f>
+        <v>21</v>
+      </c>
+      <c r="I5" s="102">
+        <f t="shared" ref="I5:I6" si="2">H5/E5</f>
+        <v>0.2413793103448276</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D6" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="E6" s="55">
+        <v>51</v>
+      </c>
+      <c r="F6" s="99">
+        <v>39</v>
+      </c>
+      <c r="G6" s="102">
+        <f t="shared" si="0"/>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="H6" s="99">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I6" s="102">
+        <f t="shared" si="2"/>
+        <v>0.23529411764705882</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="D7" s="98" t="s">
+        <v>336</v>
+      </c>
+      <c r="E7" s="100">
+        <f>E4/E6</f>
+        <v>10.392156862745098</v>
+      </c>
+      <c r="F7" s="100">
+        <f t="shared" ref="F7:H7" si="3">F4/F6</f>
+        <v>10.205128205128204</v>
+      </c>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="D8" s="98" t="s">
+        <v>335</v>
+      </c>
+      <c r="E8" s="101">
+        <f>E5/E6</f>
+        <v>1.7058823529411764</v>
+      </c>
+      <c r="F8" s="101">
+        <f t="shared" ref="F8:H8" si="4">F5/F6</f>
+        <v>1.6923076923076923</v>
+      </c>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101">
+        <f t="shared" si="4"/>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E10" s="118"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="118"/>
+      <c r="H10" s="118"/>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="118"/>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E14" s="118"/>
+      <c r="F14" s="118"/>
+      <c r="G14" s="118"/>
+      <c r="H14" s="118"/>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D15" s="96"/>
+      <c r="E15" s="96" t="s">
+        <v>233</v>
+      </c>
+      <c r="F15" s="96" t="s">
+        <v>285</v>
+      </c>
+      <c r="G15" s="96" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D16" s="34" t="s">
+        <v>413</v>
+      </c>
+      <c r="E16" s="118" t="s">
+        <v>418</v>
+      </c>
+      <c r="F16" s="97" t="s">
+        <v>420</v>
+      </c>
+      <c r="G16" s="97" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="D17" s="122" t="s">
+        <v>417</v>
+      </c>
+      <c r="E17" s="118" t="s">
+        <v>419</v>
+      </c>
+      <c r="F17" s="97" t="s">
+        <v>421</v>
+      </c>
+      <c r="G17" s="97" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D18" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="E18" s="118" t="s">
+        <v>370</v>
+      </c>
+      <c r="F18" s="97" t="s">
+        <v>372</v>
+      </c>
+      <c r="G18" s="97" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="D19" s="98" t="s">
+        <v>424</v>
+      </c>
+      <c r="E19" s="97">
+        <v>10.4</v>
+      </c>
+      <c r="F19" s="97">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="G19" s="100">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="D20" s="98" t="s">
+        <v>425</v>
+      </c>
+      <c r="E20" s="118">
+        <v>1.7</v>
+      </c>
+      <c r="F20" s="118">
+        <v>1.7</v>
+      </c>
+      <c r="G20" s="101">
+        <v>1.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03612AB4-5FBD-6E4E-8D09-BE8846D343A3}">
+  <dimension ref="A3:L29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="32.5" customWidth="1"/>
+    <col min="4" max="12" width="5.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="56" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4" s="55">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>426</v>
+      </c>
+      <c r="D4" t="s">
+        <v>382</v>
+      </c>
+      <c r="E4" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="55">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>394</v>
+      </c>
+      <c r="D5" t="s">
+        <v>426</v>
+      </c>
+      <c r="E5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6" s="55">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>429</v>
+      </c>
+      <c r="D6" t="s">
+        <v>429</v>
+      </c>
+      <c r="E6" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="55">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>431</v>
+      </c>
+      <c r="D7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E7" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="55">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>402</v>
+      </c>
+      <c r="D8" t="s">
+        <v>434</v>
+      </c>
+      <c r="E8" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="55">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>436</v>
+      </c>
+      <c r="D9" t="s">
+        <v>379</v>
+      </c>
+      <c r="E9" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="55">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>437</v>
+      </c>
+      <c r="D10" t="s">
+        <v>438</v>
+      </c>
+      <c r="E10" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="55">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>388</v>
+      </c>
+      <c r="D11" t="s">
+        <v>394</v>
+      </c>
+      <c r="E11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B12" s="55">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>439</v>
+      </c>
+      <c r="D12" t="s">
+        <v>440</v>
+      </c>
+      <c r="E12" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="57">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>441</v>
+      </c>
+      <c r="D13" t="s">
+        <v>401</v>
+      </c>
+      <c r="E13" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>469</v>
+      </c>
+      <c r="D16" t="s">
+        <v>470</v>
+      </c>
+      <c r="E16" t="s">
+        <v>466</v>
+      </c>
+      <c r="F16" t="s">
+        <v>471</v>
+      </c>
+      <c r="G16" t="s">
+        <v>472</v>
+      </c>
+      <c r="H16" t="s">
+        <v>463</v>
+      </c>
+      <c r="I16" t="s">
+        <v>473</v>
+      </c>
+      <c r="J16" t="s">
+        <v>474</v>
+      </c>
+      <c r="K16" t="s">
+        <v>475</v>
+      </c>
+      <c r="L16" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>365</v>
+      </c>
+      <c r="B17" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>426</v>
+      </c>
+      <c r="H18" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>429</v>
+      </c>
+      <c r="E19" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>480</v>
+      </c>
+      <c r="B21" t="s">
+        <v>426</v>
+      </c>
+      <c r="C21" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>429</v>
+      </c>
+      <c r="C23" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>402</v>
+      </c>
+      <c r="C25" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>437</v>
+      </c>
+      <c r="G27" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>439</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A1FD23-BDD5-C343-A786-3C7DDA226451}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>365</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573BFE4A-EE13-EF42-9710-5698F459F418}">
+  <dimension ref="B3:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD08B663-5C1A-3E4B-B727-749FBACB3D7B}">
+  <dimension ref="B2:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="64"/>
+      <c r="C3" s="65" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>300</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>328</v>
+      </c>
+      <c r="G3" s="68" t="s">
+        <v>329</v>
+      </c>
+      <c r="H3" s="69" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B4" s="123" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" s="113" t="s">
+        <v>406</v>
+      </c>
+      <c r="D4" s="72" t="s">
+        <v>445</v>
+      </c>
+      <c r="E4" s="114">
+        <v>81.61</v>
+      </c>
+      <c r="F4" s="115">
+        <v>90.25</v>
+      </c>
+      <c r="G4" s="116">
+        <v>80.290000000000006</v>
+      </c>
+      <c r="H4" s="117">
+        <v>87.27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" s="77" t="s">
+        <v>444</v>
+      </c>
+      <c r="D5" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="E5" s="104">
+        <v>83.38</v>
+      </c>
+      <c r="F5" s="105">
+        <v>90.66</v>
+      </c>
+      <c r="G5" s="93" t="s">
+        <v>443</v>
+      </c>
+      <c r="H5" s="94">
+        <v>84.24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="83" t="s">
+        <v>305</v>
+      </c>
+      <c r="C6" s="84" t="s">
+        <v>406</v>
+      </c>
+      <c r="D6" s="85" t="s">
+        <v>313</v>
+      </c>
+      <c r="E6" s="85">
+        <v>82.46</v>
+      </c>
+      <c r="F6" s="86">
+        <v>90.86</v>
+      </c>
+      <c r="G6" s="71">
+        <v>78.06</v>
+      </c>
+      <c r="H6" s="75">
+        <v>84.85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11649,10 +13071,10 @@
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
-      <c r="D2" s="118" t="s">
+      <c r="D2" s="124" t="s">
         <v>294</v>
       </c>
-      <c r="E2" s="118"/>
+      <c r="E2" s="124"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="55"/>
@@ -11665,7 +13087,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="124" t="s">
         <v>291</v>
       </c>
       <c r="C4" s="53" t="s">
@@ -11679,7 +13101,7 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="118"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="53" t="s">
         <v>293</v>
       </c>

</xml_diff>